<commit_message>
add gps data file
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,15 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7550F5-CCAC-EF49-8004-E6DAEDD8DB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B509542-747F-0446-B5F4-4DFA435CD3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="3180" yWindow="2160" windowWidth="27640" windowHeight="16940" firstSheet="2" activeTab="4" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
+    <sheet name="PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
+    <sheet name="PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
+    <sheet name="PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
+    <sheet name="PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
+    <sheet name="PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
+    <sheet name="PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
+    <sheet name="PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
+    <sheet name="PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
+    <sheet name="PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
+    <sheet name="PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
+    <sheet name="PocHistone RLFP 015" sheetId="12" r:id="rId12"/>
+    <sheet name="PocHistone RLFP 016" sheetId="13" r:id="rId13"/>
+    <sheet name="PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
+    <sheet name="PocHistone RLFP 018" sheetId="15" r:id="rId15"/>
+    <sheet name="PocHistone RLFP 019" sheetId="16" r:id="rId16"/>
+    <sheet name="PocHistone RLFP 020" sheetId="17" r:id="rId17"/>
+    <sheet name="PocHistone RLFP 021" sheetId="18" r:id="rId18"/>
+    <sheet name="PocHistone RLFP 022" sheetId="19" r:id="rId19"/>
+    <sheet name="PocHistone RLFP 023" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="384">
   <si>
     <t>A</t>
   </si>
@@ -1938,6 +1954,774 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285077F4-FC02-8F44-91B5-576823D869B3}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504A04-9B98-C942-A0B3-87EEDCC114F4}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF91483-CA2D-194B-9E9C-0698B90E3C5F}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A2B62E-D255-E642-9A27-CB767CFB6E84}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC92E7F-C385-B444-97EB-2FAF7E405F1D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA46985-9500-3F4A-B310-368C14889727}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE75D2-5269-B646-8E1B-9E77EE40A1CD}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B70E42-AAE0-7749-8639-E9DF0FAC6835}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF91C3B2-23E8-DC4F-9294-C7687C1CC223}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA4BA05-9708-2142-AEC6-D0183FE10C6D}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA186EE-C9B2-1540-8F50-36A3B503B606}">
   <dimension ref="A1:M9"/>
@@ -2312,6 +3096,99 @@
       </c>
       <c r="M9" t="s">
         <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ED1F06-122F-9544-9F84-460B1A2D95E6}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2712,8 +3589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161F0E97-0F9B-644C-96CB-34512203AC65}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,4 +3973,469 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE14A41-7155-8342-8E24-88669BBABF7F}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB2FE5C-A0B9-AF47-B279-B32862A31F23}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A79109-2A37-B641-9D62-A5F755F5CB1D}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD62516-854B-1249-A94E-9B883C3B65BF}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A32ED-889B-7C45-930B-67D659BB3C81}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add late number for rflp ID
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B509542-747F-0446-B5F4-4DFA435CD3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B1F84-2E4A-E149-88B7-16FF79A5C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2160" windowWidth="27640" windowHeight="16940" firstSheet="2" activeTab="4" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="36360" yWindow="-2440" windowWidth="22700" windowHeight="19540" firstSheet="4" activeTab="9" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="924">
   <si>
     <t>A</t>
   </si>
@@ -1207,13 +1207,1633 @@
   </si>
   <si>
     <t>P34 B12 1557</t>
+  </si>
+  <si>
+    <t>P4 D7 1825</t>
+  </si>
+  <si>
+    <t>P4 G2 1744</t>
+  </si>
+  <si>
+    <t>P4 G8 1743</t>
+  </si>
+  <si>
+    <t>P4 G9 1761</t>
+  </si>
+  <si>
+    <t>P4 H4 848</t>
+  </si>
+  <si>
+    <t>P10 A1 456</t>
+  </si>
+  <si>
+    <t>P10 B7 466</t>
+  </si>
+  <si>
+    <t>P10 D10 424</t>
+  </si>
+  <si>
+    <t>P10 E4 418</t>
+  </si>
+  <si>
+    <t>P10 E9 412</t>
+  </si>
+  <si>
+    <t>P10 E10 411</t>
+  </si>
+  <si>
+    <t>P10 E12 557</t>
+  </si>
+  <si>
+    <t>P10 F11 599</t>
+  </si>
+  <si>
+    <t>P10 G6 607</t>
+  </si>
+  <si>
+    <t>P10 H4 601</t>
+  </si>
+  <si>
+    <t>P7 E12 1561</t>
+  </si>
+  <si>
+    <t>P34 G6 1563</t>
+  </si>
+  <si>
+    <t>P7 A7 1565</t>
+  </si>
+  <si>
+    <t>P34 C1 1567</t>
+  </si>
+  <si>
+    <t>P7 C3 1569</t>
+  </si>
+  <si>
+    <t>P34 C10 1570</t>
+  </si>
+  <si>
+    <t>P7 B4 1572</t>
+  </si>
+  <si>
+    <t>P7 E1 1573</t>
+  </si>
+  <si>
+    <t>P34 G9 1575</t>
+  </si>
+  <si>
+    <t>P34 F3 1577</t>
+  </si>
+  <si>
+    <t>P34 G4 1580</t>
+  </si>
+  <si>
+    <t>P34 B8 1581</t>
+  </si>
+  <si>
+    <t>P34 C2 1582</t>
+  </si>
+  <si>
+    <t>P34 C12 1583</t>
+  </si>
+  <si>
+    <t>P34 A12 1584</t>
+  </si>
+  <si>
+    <t>P34 D3 1587</t>
+  </si>
+  <si>
+    <t>P34 D8 1590</t>
+  </si>
+  <si>
+    <t>P34 E5 1592</t>
+  </si>
+  <si>
+    <t>P34 A8 1593</t>
+  </si>
+  <si>
+    <t>P7 D11 1598</t>
+  </si>
+  <si>
+    <t>P7 D2 1599</t>
+  </si>
+  <si>
+    <t>P7 B8 1606</t>
+  </si>
+  <si>
+    <t>P7 E9 1607</t>
+  </si>
+  <si>
+    <t>P7 F5 1608</t>
+  </si>
+  <si>
+    <t>P7 C4 1610</t>
+  </si>
+  <si>
+    <t>P7 E11 1612</t>
+  </si>
+  <si>
+    <t>P7 B3 1618</t>
+  </si>
+  <si>
+    <t>P7 E6 1620</t>
+  </si>
+  <si>
+    <t>P7 D6 1621</t>
+  </si>
+  <si>
+    <t>P7 D7 1624</t>
+  </si>
+  <si>
+    <t>P34 G7 1626</t>
+  </si>
+  <si>
+    <t>P7 E3 1627</t>
+  </si>
+  <si>
+    <t>P7 D3 1628</t>
+  </si>
+  <si>
+    <t>P7 A11 1629</t>
+  </si>
+  <si>
+    <t>P7 A2 1635</t>
+  </si>
+  <si>
+    <t>P7 F9 1636</t>
+  </si>
+  <si>
+    <t>P34 E4 1638</t>
+  </si>
+  <si>
+    <t>P7 C5 1641</t>
+  </si>
+  <si>
+    <t>P7 C7 1643</t>
+  </si>
+  <si>
+    <t>P7 B10 1644</t>
+  </si>
+  <si>
+    <t>P34 B11 1645</t>
+  </si>
+  <si>
+    <t>P7 F3 1647</t>
+  </si>
+  <si>
+    <t>P4 D10 1648</t>
+  </si>
+  <si>
+    <t>P7 B9 1648</t>
+  </si>
+  <si>
+    <t>P7 B11 1649</t>
+  </si>
+  <si>
+    <t>P34 D1 1650</t>
+  </si>
+  <si>
+    <t>P4 A6 1651</t>
+  </si>
+  <si>
+    <t>P34 A10 1653</t>
+  </si>
+  <si>
+    <t>P4 C3 1654</t>
+  </si>
+  <si>
+    <t>P4 C9 1655</t>
+  </si>
+  <si>
+    <t>P34 F4 1656</t>
+  </si>
+  <si>
+    <t>P4 D1 1657</t>
+  </si>
+  <si>
+    <t>P4 B1 1658</t>
+  </si>
+  <si>
+    <t>P34 B1 1659</t>
+  </si>
+  <si>
+    <t>P34 F6 1660</t>
+  </si>
+  <si>
+    <t>P4 B10 1661</t>
+  </si>
+  <si>
+    <t>P34 E9 1662</t>
+  </si>
+  <si>
+    <t>P34 C4 1663</t>
+  </si>
+  <si>
+    <t>P34 B7 1666</t>
+  </si>
+  <si>
+    <t>P34 D4 1668</t>
+  </si>
+  <si>
+    <t>P4 C2 1671</t>
+  </si>
+  <si>
+    <t>P4 C7 1672</t>
+  </si>
+  <si>
+    <t>P34 D2 1673</t>
+  </si>
+  <si>
+    <t>P34 F7 1675</t>
+  </si>
+  <si>
+    <t>P4 C8 1676</t>
+  </si>
+  <si>
+    <t>P34 D9 1680</t>
+  </si>
+  <si>
+    <t>P4 C5 1684</t>
+  </si>
+  <si>
+    <t>P34 C6 1685</t>
+  </si>
+  <si>
+    <t>P34 B9 1686</t>
+  </si>
+  <si>
+    <t>P4 A5 1689</t>
+  </si>
+  <si>
+    <t>P4 B11 1691</t>
+  </si>
+  <si>
+    <t>P34 A9 1693</t>
+  </si>
+  <si>
+    <t>P33 B6 1700</t>
+  </si>
+  <si>
+    <t>P4 G4 1704</t>
+  </si>
+  <si>
+    <t>P33 B10 1705</t>
+  </si>
+  <si>
+    <t>P33 D5 1706</t>
+  </si>
+  <si>
+    <t>P4 F4 1709</t>
+  </si>
+  <si>
+    <t>P4 G5 1710</t>
+  </si>
+  <si>
+    <t>P34 E1 1711</t>
+  </si>
+  <si>
+    <t>P4 B8 1714</t>
+  </si>
+  <si>
+    <t>P4 A1 1715</t>
+  </si>
+  <si>
+    <t>P34 E10 1716</t>
+  </si>
+  <si>
+    <t>P4 B4 1717</t>
+  </si>
+  <si>
+    <t>P4 A11 1718</t>
+  </si>
+  <si>
+    <t>P34 G12 1724</t>
+  </si>
+  <si>
+    <t>P34 C5 1727</t>
+  </si>
+  <si>
+    <t>P4 B6 1728</t>
+  </si>
+  <si>
+    <t>P4 A2 1729</t>
+  </si>
+  <si>
+    <t>P4 B2 1730</t>
+  </si>
+  <si>
+    <t>P4 C4 1731</t>
+  </si>
+  <si>
+    <t>P34 D12 1732</t>
+  </si>
+  <si>
+    <t>P4 B9 1733</t>
+  </si>
+  <si>
+    <t>P4 B5 1734</t>
+  </si>
+  <si>
+    <t>P4 C10 1735</t>
+  </si>
+  <si>
+    <t>P4 C11 1736</t>
+  </si>
+  <si>
+    <t>P4 D3 1737</t>
+  </si>
+  <si>
+    <t>P4 D2 1738</t>
+  </si>
+  <si>
+    <t>P4 A8 1739</t>
+  </si>
+  <si>
+    <t>P4 F1 1741</t>
+  </si>
+  <si>
+    <t>P4 E11 1742</t>
+  </si>
+  <si>
+    <t>P33 D2 1746</t>
+  </si>
+  <si>
+    <t>P33 E10 1747</t>
+  </si>
+  <si>
+    <t>P4 F3 1752</t>
+  </si>
+  <si>
+    <t>P4 F6 1755</t>
+  </si>
+  <si>
+    <t>P4 D12 1757</t>
+  </si>
+  <si>
+    <t>P4 D5 1758</t>
+  </si>
+  <si>
+    <t>P4 D11 1762</t>
+  </si>
+  <si>
+    <t>P4 E4 1765</t>
+  </si>
+  <si>
+    <t>P4 E10 1767</t>
+  </si>
+  <si>
+    <t>P4 E7 1769</t>
+  </si>
+  <si>
+    <t>P33 H12 1779</t>
+  </si>
+  <si>
+    <t>P33 D6 1781</t>
+  </si>
+  <si>
+    <t>P34 H8 1784</t>
+  </si>
+  <si>
+    <t>P32 G1 1785</t>
+  </si>
+  <si>
+    <t>P33 C9 1788</t>
+  </si>
+  <si>
+    <t>P33 A7 1789</t>
+  </si>
+  <si>
+    <t>P32 H5 1790</t>
+  </si>
+  <si>
+    <t>P32 E12 1791</t>
+  </si>
+  <si>
+    <t>P33 A1 1796</t>
+  </si>
+  <si>
+    <t>P33 B7 1806</t>
+  </si>
+  <si>
+    <t>P34 H3 1807</t>
+  </si>
+  <si>
+    <t>P4 D6 1808</t>
+  </si>
+  <si>
+    <t>P33 D10 1809</t>
+  </si>
+  <si>
+    <t>P33 A10 1811</t>
+  </si>
+  <si>
+    <t>P4 F9 1812</t>
+  </si>
+  <si>
+    <t>P33 F4 1815</t>
+  </si>
+  <si>
+    <t>P33 E7 1816</t>
+  </si>
+  <si>
+    <t>P33 A4 1817</t>
+  </si>
+  <si>
+    <t>P4 E1 1818</t>
+  </si>
+  <si>
+    <t>P4 E2 1820</t>
+  </si>
+  <si>
+    <t>P4 F7 1823</t>
+  </si>
+  <si>
+    <t>P33 E1 1824</t>
+  </si>
+  <si>
+    <t>P4 G7 1828</t>
+  </si>
+  <si>
+    <t>P33 D11 1830</t>
+  </si>
+  <si>
+    <t>P33 E8 1832</t>
+  </si>
+  <si>
+    <t>P34 H11 1833</t>
+  </si>
+  <si>
+    <t>P33 A2 1834</t>
+  </si>
+  <si>
+    <t>P33 A3 1836</t>
+  </si>
+  <si>
+    <t>P4 F12 1837</t>
+  </si>
+  <si>
+    <t>P33 A12 1839</t>
+  </si>
+  <si>
+    <t>P32 F3 1840</t>
+  </si>
+  <si>
+    <t>P32 E9 1844</t>
+  </si>
+  <si>
+    <t>P32 E3 1846</t>
+  </si>
+  <si>
+    <t>P33 B4 1851</t>
+  </si>
+  <si>
+    <t>P32 E6 1857</t>
+  </si>
+  <si>
+    <t>P32 G2 1862</t>
+  </si>
+  <si>
+    <t>P32 D10 1863</t>
+  </si>
+  <si>
+    <t>P32 H6 1864</t>
+  </si>
+  <si>
+    <t>P32 D11 1864</t>
+  </si>
+  <si>
+    <t>P32 G10 1865</t>
+  </si>
+  <si>
+    <t>P32 G12 1874</t>
+  </si>
+  <si>
+    <t>P32 F9 1875</t>
+  </si>
+  <si>
+    <t>P32 H2 1876</t>
+  </si>
+  <si>
+    <t>P32 F6 1877</t>
+  </si>
+  <si>
+    <t>P32 F12 1883</t>
+  </si>
+  <si>
+    <t>P32 D9 1884</t>
+  </si>
+  <si>
+    <t>P33 H11 1886</t>
+  </si>
+  <si>
+    <t>P32 D7 1891</t>
+  </si>
+  <si>
+    <t>P36 E8 1896</t>
+  </si>
+  <si>
+    <t>P33 G6 1900</t>
+  </si>
+  <si>
+    <t>P36 E7 1901</t>
+  </si>
+  <si>
+    <t>P35 H10 1902</t>
+  </si>
+  <si>
+    <t>P35 H3 1906</t>
+  </si>
+  <si>
+    <t>P36 E10 1907</t>
+  </si>
+  <si>
+    <t>P36 D1 1915</t>
+  </si>
+  <si>
+    <t>P32 D2 1917</t>
+  </si>
+  <si>
+    <t>P36 B6 1918</t>
+  </si>
+  <si>
+    <t>P36 C10 1919</t>
+  </si>
+  <si>
+    <t>P35 H6 1922</t>
+  </si>
+  <si>
+    <t>P36 C7 1926</t>
+  </si>
+  <si>
+    <t>P36 E4 1927</t>
+  </si>
+  <si>
+    <t>P36 B7 1930</t>
+  </si>
+  <si>
+    <t>P33 G11 1931</t>
+  </si>
+  <si>
+    <t>P36 D10 1933</t>
+  </si>
+  <si>
+    <t>P32 C11 1934</t>
+  </si>
+  <si>
+    <t>P32 B8 1937</t>
+  </si>
+  <si>
+    <t>P32 G7 1939</t>
+  </si>
+  <si>
+    <t>P32 H9 1940</t>
+  </si>
+  <si>
+    <t>P34 H10 1942</t>
+  </si>
+  <si>
+    <t>P33 F10 1944</t>
+  </si>
+  <si>
+    <t>P32 H11 1945</t>
+  </si>
+  <si>
+    <t>P32 H12 1949</t>
+  </si>
+  <si>
+    <t>P32 D6 1953</t>
+  </si>
+  <si>
+    <t>P32 G11 1954</t>
+  </si>
+  <si>
+    <t>P32 F10 1955</t>
+  </si>
+  <si>
+    <t>P33 B11 1958</t>
+  </si>
+  <si>
+    <t>P33 D11 1958</t>
+  </si>
+  <si>
+    <t>P36 D11 1960</t>
+  </si>
+  <si>
+    <t>P36 D7 1965</t>
+  </si>
+  <si>
+    <t>P32 C10 1969</t>
+  </si>
+  <si>
+    <t>P33 G10 1970</t>
+  </si>
+  <si>
+    <t>P32 B2 1971</t>
+  </si>
+  <si>
+    <t>P36 B2 1973</t>
+  </si>
+  <si>
+    <t>P32 C1 1975</t>
+  </si>
+  <si>
+    <t>P35 H2 1976</t>
+  </si>
+  <si>
+    <t>P36 C4 1980</t>
+  </si>
+  <si>
+    <t>P32 D3 1986</t>
+  </si>
+  <si>
+    <t>P33 G9 1987</t>
+  </si>
+  <si>
+    <t>P33 G2 1989</t>
+  </si>
+  <si>
+    <t>P32 A8 1990</t>
+  </si>
+  <si>
+    <t>P35 G6 1991</t>
+  </si>
+  <si>
+    <t>P36 A7 1992</t>
+  </si>
+  <si>
+    <t>P32 C4 1993</t>
+  </si>
+  <si>
+    <t>P32 B6 1995</t>
+  </si>
+  <si>
+    <t>P35 H9 1998</t>
+  </si>
+  <si>
+    <t>P32 C6 1999</t>
+  </si>
+  <si>
+    <t>P32 B10 2000</t>
+  </si>
+  <si>
+    <t>P32 C3 2001</t>
+  </si>
+  <si>
+    <t>P32 A9 2003</t>
+  </si>
+  <si>
+    <t>P33 F12 2004</t>
+  </si>
+  <si>
+    <t>P35 H5 2007</t>
+  </si>
+  <si>
+    <t>P36 C6 2008</t>
+  </si>
+  <si>
+    <t>P36 B4 2009</t>
+  </si>
+  <si>
+    <t>P36 D6 2010</t>
+  </si>
+  <si>
+    <t>P35 H8 2015</t>
+  </si>
+  <si>
+    <t>P36 C11 2017</t>
+  </si>
+  <si>
+    <t>P33 G4 2019</t>
+  </si>
+  <si>
+    <t>P36 C8 2022</t>
+  </si>
+  <si>
+    <t>P32 C12 2023</t>
+  </si>
+  <si>
+    <t>P32 A10 2024</t>
+  </si>
+  <si>
+    <t>P36 D5 2026</t>
+  </si>
+  <si>
+    <t>P19 D9 2029</t>
+  </si>
+  <si>
+    <t>P19 F1 2030</t>
+  </si>
+  <si>
+    <t>P19 G1 2032</t>
+  </si>
+  <si>
+    <t>P19 F7 2033</t>
+  </si>
+  <si>
+    <t>P19 E4 2035</t>
+  </si>
+  <si>
+    <t>P19 E8 2036</t>
+  </si>
+  <si>
+    <t>P19 F8 2038</t>
+  </si>
+  <si>
+    <t>P19 E3 2039</t>
+  </si>
+  <si>
+    <t>P19 D6 2041</t>
+  </si>
+  <si>
+    <t>P19 F2 2043</t>
+  </si>
+  <si>
+    <t>P16 E4 2048</t>
+  </si>
+  <si>
+    <t>P16 A9 2050</t>
+  </si>
+  <si>
+    <t>P19 G3 2053</t>
+  </si>
+  <si>
+    <t>P16 C9 2054</t>
+  </si>
+  <si>
+    <t>P16 E5 2055</t>
+  </si>
+  <si>
+    <t>P16 F8 2056</t>
+  </si>
+  <si>
+    <t>P16 C11 2060</t>
+  </si>
+  <si>
+    <t>P16 B8 2061</t>
+  </si>
+  <si>
+    <t>P16 A12 2064</t>
+  </si>
+  <si>
+    <t>P16 D4 2070</t>
+  </si>
+  <si>
+    <t>P16 E9 2071</t>
+  </si>
+  <si>
+    <t>P16 C5 2072</t>
+  </si>
+  <si>
+    <t>P16 E12 2073</t>
+  </si>
+  <si>
+    <t>P16 B9 2077</t>
+  </si>
+  <si>
+    <t>P28 D12 2081</t>
+  </si>
+  <si>
+    <t>P18 A11 2082</t>
+  </si>
+  <si>
+    <t>P32 B1 2085</t>
+  </si>
+  <si>
+    <t>P32 C7 2086</t>
+  </si>
+  <si>
+    <t>P32 B7 2087</t>
+  </si>
+  <si>
+    <t>P36 E6 2092</t>
+  </si>
+  <si>
+    <t>P19 D5 2094</t>
+  </si>
+  <si>
+    <t>P36 E11 2098</t>
+  </si>
+  <si>
+    <t>P36 E3 2099</t>
+  </si>
+  <si>
+    <t>P17 D11 2101</t>
+  </si>
+  <si>
+    <t>P17 F3 2102</t>
+  </si>
+  <si>
+    <t>P22 A2 2105</t>
+  </si>
+  <si>
+    <t>P19 H11 2111</t>
+  </si>
+  <si>
+    <t>P18 H8 2115</t>
+  </si>
+  <si>
+    <t>P19 H3 2116</t>
+  </si>
+  <si>
+    <t>P21 B11 2118</t>
+  </si>
+  <si>
+    <t>P21 B2 2119</t>
+  </si>
+  <si>
+    <t>P21 B6 2120</t>
+  </si>
+  <si>
+    <t>P21 A4 2121</t>
+  </si>
+  <si>
+    <t>P21 A7 2129</t>
+  </si>
+  <si>
+    <t>P18 H4 2130</t>
+  </si>
+  <si>
+    <t>P21 B7 2131</t>
+  </si>
+  <si>
+    <t>P19 G7 2132</t>
+  </si>
+  <si>
+    <t>P19 H9 2134</t>
+  </si>
+  <si>
+    <t>P19 H1 2135</t>
+  </si>
+  <si>
+    <t>P22 A1 2136</t>
+  </si>
+  <si>
+    <t>P21 A1 2137</t>
+  </si>
+  <si>
+    <t>P19 H2 2139</t>
+  </si>
+  <si>
+    <t>P18 H7 2140</t>
+  </si>
+  <si>
+    <t>P19 H5 2143</t>
+  </si>
+  <si>
+    <t>P21 A3 2144</t>
+  </si>
+  <si>
+    <t>P21 B4 2145</t>
+  </si>
+  <si>
+    <t>P21 A2 2146</t>
+  </si>
+  <si>
+    <t>P18 H9 2147</t>
+  </si>
+  <si>
+    <t>P19 H8 2149</t>
+  </si>
+  <si>
+    <t>P17 C6 2150</t>
+  </si>
+  <si>
+    <t>P19 H10 2156</t>
+  </si>
+  <si>
+    <t>P21 B5 2157</t>
+  </si>
+  <si>
+    <t>P19 G8 2158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P19 G4 2159 </t>
+  </si>
+  <si>
+    <t>P18 D9 2168</t>
+  </si>
+  <si>
+    <t>P18 H12 2170</t>
+  </si>
+  <si>
+    <t>P19 F10 2172</t>
+  </si>
+  <si>
+    <t>P19 F3 2175</t>
+  </si>
+  <si>
+    <t>P16 A5 2176</t>
+  </si>
+  <si>
+    <t>P16 E8 2177</t>
+  </si>
+  <si>
+    <t>P17 G5 2181</t>
+  </si>
+  <si>
+    <t>P16 E11 2183</t>
+  </si>
+  <si>
+    <t>P16 E3 2184</t>
+  </si>
+  <si>
+    <t>P16 E1 2185</t>
+  </si>
+  <si>
+    <t>P16 C2 2186</t>
+  </si>
+  <si>
+    <t>P16 C1 2189</t>
+  </si>
+  <si>
+    <t>P16 B12 2190</t>
+  </si>
+  <si>
+    <t>P16 D3 2192</t>
+  </si>
+  <si>
+    <t>P16 C10 2195</t>
+  </si>
+  <si>
+    <t>P16 A7 2196</t>
+  </si>
+  <si>
+    <t>P16 F11 2197</t>
+  </si>
+  <si>
+    <t>P16 A10 2202</t>
+  </si>
+  <si>
+    <t>P16 F1 2205</t>
+  </si>
+  <si>
+    <t>P16 D8 2206</t>
+  </si>
+  <si>
+    <t>P16 B5 2208</t>
+  </si>
+  <si>
+    <t>P16 F2 2213</t>
+  </si>
+  <si>
+    <t>P16 F12 2214</t>
+  </si>
+  <si>
+    <t>P16 B4 2219</t>
+  </si>
+  <si>
+    <t>P16 B10 2221</t>
+  </si>
+  <si>
+    <t>P16 D11 2225</t>
+  </si>
+  <si>
+    <t>P19 E10 2226</t>
+  </si>
+  <si>
+    <t>P19 G10 2227</t>
+  </si>
+  <si>
+    <t>P19 H4 2228</t>
+  </si>
+  <si>
+    <t>P19 E2 2230</t>
+  </si>
+  <si>
+    <t>P19 E5 2234</t>
+  </si>
+  <si>
+    <t>P19 E7 2235</t>
+  </si>
+  <si>
+    <t>P19 F5 2236</t>
+  </si>
+  <si>
+    <t>P18 G6 2237</t>
+  </si>
+  <si>
+    <t>P19 E11 2238</t>
+  </si>
+  <si>
+    <t>P19 G2 2239</t>
+  </si>
+  <si>
+    <t>P18 E4 2240</t>
+  </si>
+  <si>
+    <t>P18 G10 2241</t>
+  </si>
+  <si>
+    <t>P17 D8 2242</t>
+  </si>
+  <si>
+    <t>P17 C11 2244</t>
+  </si>
+  <si>
+    <t>P18 D4 2246</t>
+  </si>
+  <si>
+    <t>P17 E11 2247</t>
+  </si>
+  <si>
+    <t>P18 F7 2248</t>
+  </si>
+  <si>
+    <t>P17 E6 2249</t>
+  </si>
+  <si>
+    <t>P17 E10 2252</t>
+  </si>
+  <si>
+    <t>P18 E2 2256</t>
+  </si>
+  <si>
+    <t>P18 E1 2259</t>
+  </si>
+  <si>
+    <t>P17 D4 2260</t>
+  </si>
+  <si>
+    <t>P17 C10 2261</t>
+  </si>
+  <si>
+    <t>P17 C4 2262</t>
+  </si>
+  <si>
+    <t>P17 E8 2263</t>
+  </si>
+  <si>
+    <t>P17 C9 2264</t>
+  </si>
+  <si>
+    <t>P17 F2 2266</t>
+  </si>
+  <si>
+    <t>P17 E5 2267</t>
+  </si>
+  <si>
+    <t>P18 G3 2272</t>
+  </si>
+  <si>
+    <t>P17 D5 2273</t>
+  </si>
+  <si>
+    <t>P18 E10 2274</t>
+  </si>
+  <si>
+    <t>P18 F4 2276</t>
+  </si>
+  <si>
+    <t>P17 E4 2277</t>
+  </si>
+  <si>
+    <t>P18 H3 2278</t>
+  </si>
+  <si>
+    <t>P18 E9 2279</t>
+  </si>
+  <si>
+    <t>P17 C12 2280</t>
+  </si>
+  <si>
+    <t>P17 C8 2281</t>
+  </si>
+  <si>
+    <t>P17 D3 2283</t>
+  </si>
+  <si>
+    <t>P18 E8 2285</t>
+  </si>
+  <si>
+    <t>P18 G4 2286</t>
+  </si>
+  <si>
+    <t>P18 G8 2287</t>
+  </si>
+  <si>
+    <t>P18 G9 2288</t>
+  </si>
+  <si>
+    <t>P18 G12 2289</t>
+  </si>
+  <si>
+    <t>P18 D3 2290</t>
+  </si>
+  <si>
+    <t>P18 D5 2291</t>
+  </si>
+  <si>
+    <t>P17 D2 2292</t>
+  </si>
+  <si>
+    <t>P17 E1 2294</t>
+  </si>
+  <si>
+    <t>P18 D7 2299</t>
+  </si>
+  <si>
+    <t>P18 H1 2300</t>
+  </si>
+  <si>
+    <t>P18 H2 2301</t>
+  </si>
+  <si>
+    <t>P18 F6 2302</t>
+  </si>
+  <si>
+    <t>P18 D2 2303</t>
+  </si>
+  <si>
+    <t>P17 D7 2306</t>
+  </si>
+  <si>
+    <t>P18 E7 2309</t>
+  </si>
+  <si>
+    <t>P17 E12 2310</t>
+  </si>
+  <si>
+    <t>P18 D1 2319</t>
+  </si>
+  <si>
+    <t>P18 D10 2321</t>
+  </si>
+  <si>
+    <t>P17 E9 2322</t>
+  </si>
+  <si>
+    <t>P18 F9 2323</t>
+  </si>
+  <si>
+    <t>P18 D8 2324</t>
+  </si>
+  <si>
+    <t>P18 C9 2328</t>
+  </si>
+  <si>
+    <t>P28 H10 2332</t>
+  </si>
+  <si>
+    <t>P29 H5 2335</t>
+  </si>
+  <si>
+    <t>P18 B10 2336</t>
+  </si>
+  <si>
+    <t>P18 C6 2337</t>
+  </si>
+  <si>
+    <t>P29 H2 2338</t>
+  </si>
+  <si>
+    <t>P28 E1 2339</t>
+  </si>
+  <si>
+    <t>P17 H7 2340</t>
+  </si>
+  <si>
+    <t>P18 B12 2343</t>
+  </si>
+  <si>
+    <t>P28 E2 2345</t>
+  </si>
+  <si>
+    <t>P28 H11 2346</t>
+  </si>
+  <si>
+    <t>P29 F10 2348</t>
+  </si>
+  <si>
+    <t>P18 A2 2352</t>
+  </si>
+  <si>
+    <t>P29 H7 2356</t>
+  </si>
+  <si>
+    <t>P18 A9 2357</t>
+  </si>
+  <si>
+    <t>P17 G10 2358</t>
+  </si>
+  <si>
+    <t>P29 G1 2359</t>
+  </si>
+  <si>
+    <t>P18 B5 2360</t>
+  </si>
+  <si>
+    <t>P28 G3 2362</t>
+  </si>
+  <si>
+    <t>P18 C5 2367</t>
+  </si>
+  <si>
+    <t>P29 G10 2368</t>
+  </si>
+  <si>
+    <t>P18 C8 2371</t>
+  </si>
+  <si>
+    <t>P28 E9 2372</t>
+  </si>
+  <si>
+    <t>P17 H12 2374</t>
+  </si>
+  <si>
+    <t>P28 G4 2376</t>
+  </si>
+  <si>
+    <t>P18 C7 2378</t>
+  </si>
+  <si>
+    <t>P29 G6 2381</t>
+  </si>
+  <si>
+    <t>P18 C4 2383</t>
+  </si>
+  <si>
+    <t>P29 G4 2384</t>
+  </si>
+  <si>
+    <t>P28 F10 2387</t>
+  </si>
+  <si>
+    <t>P28 G2 2388</t>
+  </si>
+  <si>
+    <t>P28 E12 2389</t>
+  </si>
+  <si>
+    <t>P29 F12 2390</t>
+  </si>
+  <si>
+    <t>P28 E7 2391</t>
+  </si>
+  <si>
+    <t>P28 H8 2392</t>
+  </si>
+  <si>
+    <t>P18 A12 2393</t>
+  </si>
+  <si>
+    <t>P29 H9 2394</t>
+  </si>
+  <si>
+    <t>P28 F7 2396</t>
+  </si>
+  <si>
+    <t>P29 F6 2397</t>
+  </si>
+  <si>
+    <t>P28 E3 2398</t>
+  </si>
+  <si>
+    <t>P18 C10 2400</t>
+  </si>
+  <si>
+    <t>P28 G10 2401</t>
+  </si>
+  <si>
+    <t>P29 G3 2402</t>
+  </si>
+  <si>
+    <t>P29 H4 2403</t>
+  </si>
+  <si>
+    <t>P28 H2 2404</t>
+  </si>
+  <si>
+    <t>P29 G2 2405</t>
+  </si>
+  <si>
+    <t>P28 E11 2406</t>
+  </si>
+  <si>
+    <t>P29 G7 2407</t>
+  </si>
+  <si>
+    <t>P29 G12 2408</t>
+  </si>
+  <si>
+    <t>P18 C12 2413</t>
+  </si>
+  <si>
+    <t>P18 B9 2414</t>
+  </si>
+  <si>
+    <t>P17 G8 2415</t>
+  </si>
+  <si>
+    <t>P17 H3 2416</t>
+  </si>
+  <si>
+    <t>P29 G9 2417</t>
+  </si>
+  <si>
+    <t>P17 H11 2419</t>
+  </si>
+  <si>
+    <t>P28 G12 2420</t>
+  </si>
+  <si>
+    <t>P17 H6 2423</t>
+  </si>
+  <si>
+    <t>P18 B7 2424</t>
+  </si>
+  <si>
+    <t>P28 E8 2425</t>
+  </si>
+  <si>
+    <t>P28 E12 2427</t>
+  </si>
+  <si>
+    <t>P29 F7 2428</t>
+  </si>
+  <si>
+    <t>P18 C3 2429</t>
+  </si>
+  <si>
+    <t>P28 G8 2430</t>
+  </si>
+  <si>
+    <t>P28 E4 2432</t>
+  </si>
+  <si>
+    <t>P28 H6 2433</t>
+  </si>
+  <si>
+    <t>P29 H3 2434</t>
+  </si>
+  <si>
+    <t>P29 H1 2440</t>
+  </si>
+  <si>
+    <t>P29 G11 2441</t>
+  </si>
+  <si>
+    <t>P28 E5 2445</t>
+  </si>
+  <si>
+    <t>P28 F9 2448</t>
+  </si>
+  <si>
+    <t>P28 H12 2449</t>
+  </si>
+  <si>
+    <t>P28 G11 2452</t>
+  </si>
+  <si>
+    <t>P18 A7 2453</t>
+  </si>
+  <si>
+    <t>P18 A8 2454</t>
+  </si>
+  <si>
+    <t>P25 H11 2460</t>
+  </si>
+  <si>
+    <t>P30 H6 2461</t>
+  </si>
+  <si>
+    <t>P20 B1 2463</t>
+  </si>
+  <si>
+    <t>P29 B4 2464</t>
+  </si>
+  <si>
+    <t>P29 A9 2465</t>
+  </si>
+  <si>
+    <t>P20 A8 2466</t>
+  </si>
+  <si>
+    <t>P29 C6 2469</t>
+  </si>
+  <si>
+    <t>P29 E4 2470</t>
+  </si>
+  <si>
+    <t>P29 A2 2471</t>
+  </si>
+  <si>
+    <t>P29 D7 2472</t>
+  </si>
+  <si>
+    <t>P29 A10 2473</t>
+  </si>
+  <si>
+    <t>P29 A5 2474</t>
+  </si>
+  <si>
+    <t>P29 E8 2476</t>
+  </si>
+  <si>
+    <t>P29 C2 2477</t>
+  </si>
+  <si>
+    <t>P30 H7 2478</t>
+  </si>
+  <si>
+    <t>P29 D8 2479</t>
+  </si>
+  <si>
+    <t>P29 C11 2480</t>
+  </si>
+  <si>
+    <t>P29 D6 2482</t>
+  </si>
+  <si>
+    <t>P29 C5 2487</t>
+  </si>
+  <si>
+    <t>P29 C4 2489</t>
+  </si>
+  <si>
+    <t>P30 H2 2491</t>
+  </si>
+  <si>
+    <t>P29 B7 2494</t>
+  </si>
+  <si>
+    <t>P29 B12 2495</t>
+  </si>
+  <si>
+    <t>P29 E2 2499</t>
+  </si>
+  <si>
+    <t>P30 H12 2500</t>
+  </si>
+  <si>
+    <t>P30 G11 2502</t>
+  </si>
+  <si>
+    <t>P25 E12 2503</t>
+  </si>
+  <si>
+    <t>P25 F12 2504</t>
+  </si>
+  <si>
+    <t>P29 E12 2506</t>
+  </si>
+  <si>
+    <t>P14 D7 2507</t>
+  </si>
+  <si>
+    <t>P23 A11 2509</t>
+  </si>
+  <si>
+    <t>P14 C5 2510</t>
+  </si>
+  <si>
+    <t>P14 D11 2511</t>
+  </si>
+  <si>
+    <t>P14 D8 2512</t>
+  </si>
+  <si>
+    <t>P14 D4 2513</t>
+  </si>
+  <si>
+    <t>P24 C11 2520</t>
+  </si>
+  <si>
+    <t>P14 C10 2524</t>
+  </si>
+  <si>
+    <t>P26 B5 2534</t>
+  </si>
+  <si>
+    <t>P27 G3 2535</t>
+  </si>
+  <si>
+    <t>P27 F10 2538</t>
+  </si>
+  <si>
+    <t>P24 C2 2540</t>
+  </si>
+  <si>
+    <t>P14 D6 2542</t>
+  </si>
+  <si>
+    <t>P14 C12 2546</t>
+  </si>
+  <si>
+    <t>P14 C9 2547</t>
+  </si>
+  <si>
+    <t>P14 C2 2549</t>
+  </si>
+  <si>
+    <t>P14 B11 2550</t>
+  </si>
+  <si>
+    <t>P14 D10 2551</t>
+  </si>
+  <si>
+    <t>P30 E9 2553</t>
+  </si>
+  <si>
+    <t>P30 C11 2554</t>
+  </si>
+  <si>
+    <t>P30 C6 2555</t>
+  </si>
+  <si>
+    <t>P30 D4 2557</t>
+  </si>
+  <si>
+    <t>P24 E11 2567</t>
+  </si>
+  <si>
+    <t>P25 F3 2570</t>
+  </si>
+  <si>
+    <t>P25 H2 2571</t>
+  </si>
+  <si>
+    <t>P25 H6 2572</t>
+  </si>
+  <si>
+    <t>P24 G5 2577</t>
+  </si>
+  <si>
+    <t>P25 H3 2581</t>
+  </si>
+  <si>
+    <t>P24 H1 2584</t>
+  </si>
+  <si>
+    <t>P24 G7 2585</t>
+  </si>
+  <si>
+    <t>P25 E11 2586</t>
+  </si>
+  <si>
+    <t>P24 G12 2588</t>
+  </si>
+  <si>
+    <t>P24 H2 2590</t>
+  </si>
+  <si>
+    <t>P24 F6 2591</t>
+  </si>
+  <si>
+    <t>P24 H10 2593</t>
+  </si>
+  <si>
+    <t>P25 F1 2594</t>
+  </si>
+  <si>
+    <t>P25 F9 2596</t>
+  </si>
+  <si>
+    <t>P24 E9 2598</t>
+  </si>
+  <si>
+    <t>P24 H11 2599</t>
+  </si>
+  <si>
+    <t>P25 G8 2601</t>
+  </si>
+  <si>
+    <t>P29 E10 2603</t>
+  </si>
+  <si>
+    <t>P29 E7 2607</t>
+  </si>
+  <si>
+    <t>P29 D9 2608</t>
+  </si>
+  <si>
+    <t>P29 E3 2610</t>
+  </si>
+  <si>
+    <t>P29 D4 2611</t>
+  </si>
+  <si>
+    <t>P30 G10 2612</t>
+  </si>
+  <si>
+    <t>P29 C9 2614</t>
+  </si>
+  <si>
+    <t>P29 B6 2615</t>
+  </si>
+  <si>
+    <t>P29 D11 2616</t>
+  </si>
+  <si>
+    <t>P30 B7 2619</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P30 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1221,13 +2841,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1242,8 +2874,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1958,11 +3593,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285077F4-FC02-8F44-91B5-576823D869B3}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -2006,35 +3650,254 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>853</v>
+      </c>
+      <c r="C2" t="s">
+        <v>854</v>
+      </c>
+      <c r="D2" t="s">
+        <v>855</v>
+      </c>
+      <c r="E2" t="s">
+        <v>856</v>
+      </c>
+      <c r="F2" t="s">
+        <v>857</v>
+      </c>
+      <c r="G2" t="s">
+        <v>858</v>
+      </c>
+      <c r="H2" t="s">
+        <v>859</v>
+      </c>
+      <c r="I2" t="s">
+        <v>860</v>
+      </c>
+      <c r="J2" t="s">
+        <v>861</v>
+      </c>
+      <c r="K2" t="s">
+        <v>862</v>
+      </c>
+      <c r="L2" t="s">
+        <v>863</v>
+      </c>
+      <c r="M2" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>865</v>
+      </c>
+      <c r="C3" t="s">
+        <v>866</v>
+      </c>
+      <c r="D3" t="s">
+        <v>867</v>
+      </c>
+      <c r="E3" t="s">
+        <v>868</v>
+      </c>
+      <c r="F3" t="s">
+        <v>869</v>
+      </c>
+      <c r="G3" t="s">
+        <v>870</v>
+      </c>
+      <c r="H3" t="s">
+        <v>871</v>
+      </c>
+      <c r="I3" t="s">
+        <v>872</v>
+      </c>
+      <c r="J3" t="s">
+        <v>873</v>
+      </c>
+      <c r="K3" t="s">
+        <v>874</v>
+      </c>
+      <c r="L3" t="s">
+        <v>875</v>
+      </c>
+      <c r="M3" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>877</v>
+      </c>
+      <c r="C4" t="s">
+        <v>878</v>
+      </c>
+      <c r="D4" t="s">
+        <v>879</v>
+      </c>
+      <c r="E4" t="s">
+        <v>880</v>
+      </c>
+      <c r="F4" t="s">
+        <v>881</v>
+      </c>
+      <c r="G4" t="s">
+        <v>882</v>
+      </c>
+      <c r="H4" t="s">
+        <v>883</v>
+      </c>
+      <c r="I4" t="s">
+        <v>884</v>
+      </c>
+      <c r="J4" t="s">
+        <v>885</v>
+      </c>
+      <c r="K4" t="s">
+        <v>886</v>
+      </c>
+      <c r="L4" t="s">
+        <v>887</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>888</v>
+      </c>
+      <c r="C5" t="s">
+        <v>889</v>
+      </c>
+      <c r="D5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E5" t="s">
+        <v>891</v>
+      </c>
+      <c r="F5" t="s">
+        <v>892</v>
+      </c>
+      <c r="G5" t="s">
+        <v>893</v>
+      </c>
+      <c r="H5" t="s">
+        <v>894</v>
+      </c>
+      <c r="I5" t="s">
+        <v>895</v>
+      </c>
+      <c r="J5" t="s">
+        <v>896</v>
+      </c>
+      <c r="K5" t="s">
+        <v>897</v>
+      </c>
+      <c r="L5" t="s">
+        <v>898</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>899</v>
+      </c>
+      <c r="C6" t="s">
+        <v>900</v>
+      </c>
+      <c r="D6" t="s">
+        <v>901</v>
+      </c>
+      <c r="E6" t="s">
+        <v>902</v>
+      </c>
+      <c r="F6" t="s">
+        <v>903</v>
+      </c>
+      <c r="G6" t="s">
+        <v>904</v>
+      </c>
+      <c r="H6" t="s">
+        <v>905</v>
+      </c>
+      <c r="I6" t="s">
+        <v>906</v>
+      </c>
+      <c r="J6" t="s">
+        <v>907</v>
+      </c>
+      <c r="K6" t="s">
+        <v>908</v>
+      </c>
+      <c r="L6" t="s">
+        <v>909</v>
+      </c>
+      <c r="M6" t="s">
+        <v>910</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>911</v>
+      </c>
+      <c r="C7" t="s">
+        <v>912</v>
+      </c>
+      <c r="D7" t="s">
+        <v>913</v>
+      </c>
+      <c r="E7" t="s">
+        <v>914</v>
+      </c>
+      <c r="F7" t="s">
+        <v>915</v>
+      </c>
+      <c r="G7" t="s">
+        <v>916</v>
+      </c>
+      <c r="H7" t="s">
+        <v>917</v>
+      </c>
+      <c r="I7" t="s">
+        <v>918</v>
+      </c>
+      <c r="J7" t="s">
+        <v>919</v>
+      </c>
+      <c r="K7" t="s">
+        <v>920</v>
+      </c>
+      <c r="L7" t="s">
+        <v>921</v>
+      </c>
+      <c r="M7" t="s">
+        <v>922</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -3590,7 +5453,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3979,11 +5842,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE14A41-7155-8342-8E24-88669BBABF7F}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4027,40 +5897,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G4" t="s">
+        <v>411</v>
+      </c>
+      <c r="H4" t="s">
+        <v>412</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5" t="s">
+        <v>419</v>
+      </c>
+      <c r="D5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F5" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" t="s">
+        <v>423</v>
+      </c>
+      <c r="H5" t="s">
+        <v>424</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>430</v>
+      </c>
+      <c r="C6" t="s">
+        <v>431</v>
+      </c>
+      <c r="D6" t="s">
+        <v>432</v>
+      </c>
+      <c r="E6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F6" t="s">
+        <v>434</v>
+      </c>
+      <c r="G6" t="s">
+        <v>435</v>
+      </c>
+      <c r="H6" t="s">
+        <v>436</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>442</v>
+      </c>
+      <c r="C7" t="s">
+        <v>443</v>
+      </c>
+      <c r="D7" t="s">
+        <v>444</v>
+      </c>
+      <c r="E7" t="s">
+        <v>445</v>
+      </c>
+      <c r="F7" t="s">
+        <v>446</v>
+      </c>
+      <c r="G7" t="s">
+        <v>447</v>
+      </c>
+      <c r="H7" t="s">
+        <v>448</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C8" t="s">
+        <v>455</v>
+      </c>
+      <c r="D8" t="s">
+        <v>456</v>
+      </c>
+      <c r="E8" t="s">
+        <v>457</v>
+      </c>
+      <c r="F8" t="s">
+        <v>458</v>
+      </c>
+      <c r="G8" t="s">
+        <v>459</v>
+      </c>
+      <c r="H8" t="s">
+        <v>460</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C9" t="s">
+        <v>467</v>
+      </c>
+      <c r="D9" t="s">
+        <v>468</v>
+      </c>
+      <c r="E9" t="s">
+        <v>469</v>
+      </c>
+      <c r="F9" t="s">
+        <v>470</v>
+      </c>
+      <c r="G9" t="s">
+        <v>471</v>
+      </c>
+      <c r="H9" t="s">
+        <v>472</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -4073,10 +6231,19 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4120,40 +6287,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E2" t="s">
+        <v>481</v>
+      </c>
+      <c r="F2" t="s">
+        <v>482</v>
+      </c>
+      <c r="G2" t="s">
+        <v>483</v>
+      </c>
+      <c r="H2" t="s">
+        <v>484</v>
+      </c>
+      <c r="I2" t="s">
+        <v>485</v>
+      </c>
+      <c r="J2" t="s">
+        <v>486</v>
+      </c>
+      <c r="K2" t="s">
+        <v>487</v>
+      </c>
+      <c r="L2" t="s">
+        <v>488</v>
+      </c>
+      <c r="M2" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D3" t="s">
+        <v>492</v>
+      </c>
+      <c r="E3" t="s">
+        <v>493</v>
+      </c>
+      <c r="F3" t="s">
+        <v>494</v>
+      </c>
+      <c r="G3" t="s">
+        <v>495</v>
+      </c>
+      <c r="H3" t="s">
+        <v>496</v>
+      </c>
+      <c r="I3" t="s">
+        <v>497</v>
+      </c>
+      <c r="J3" t="s">
+        <v>498</v>
+      </c>
+      <c r="K3" t="s">
+        <v>499</v>
+      </c>
+      <c r="L3" t="s">
+        <v>500</v>
+      </c>
+      <c r="M3" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>502</v>
+      </c>
+      <c r="D4" t="s">
+        <v>503</v>
+      </c>
+      <c r="E4" t="s">
+        <v>504</v>
+      </c>
+      <c r="F4" t="s">
+        <v>505</v>
+      </c>
+      <c r="G4" t="s">
+        <v>506</v>
+      </c>
+      <c r="H4" t="s">
+        <v>507</v>
+      </c>
+      <c r="I4" t="s">
+        <v>508</v>
+      </c>
+      <c r="J4" t="s">
+        <v>509</v>
+      </c>
+      <c r="K4" t="s">
+        <v>510</v>
+      </c>
+      <c r="L4" t="s">
+        <v>511</v>
+      </c>
+      <c r="M4" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>513</v>
+      </c>
+      <c r="D5" t="s">
+        <v>514</v>
+      </c>
+      <c r="E5" t="s">
+        <v>515</v>
+      </c>
+      <c r="F5" t="s">
+        <v>516</v>
+      </c>
+      <c r="G5" t="s">
+        <v>517</v>
+      </c>
+      <c r="H5" t="s">
+        <v>518</v>
+      </c>
+      <c r="I5" t="s">
+        <v>519</v>
+      </c>
+      <c r="J5" t="s">
+        <v>520</v>
+      </c>
+      <c r="K5" t="s">
+        <v>521</v>
+      </c>
+      <c r="L5" t="s">
+        <v>522</v>
+      </c>
+      <c r="M5" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C6" t="s">
+        <v>525</v>
+      </c>
+      <c r="D6" t="s">
+        <v>526</v>
+      </c>
+      <c r="E6" t="s">
+        <v>527</v>
+      </c>
+      <c r="F6" t="s">
+        <v>528</v>
+      </c>
+      <c r="G6" t="s">
+        <v>529</v>
+      </c>
+      <c r="H6" t="s">
+        <v>530</v>
+      </c>
+      <c r="I6" t="s">
+        <v>531</v>
+      </c>
+      <c r="J6" t="s">
+        <v>532</v>
+      </c>
+      <c r="K6" t="s">
+        <v>532</v>
+      </c>
+      <c r="L6" t="s">
+        <v>533</v>
+      </c>
+      <c r="M6" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>535</v>
+      </c>
+      <c r="C7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D7" t="s">
+        <v>537</v>
+      </c>
+      <c r="E7" t="s">
+        <v>538</v>
+      </c>
+      <c r="F7" t="s">
+        <v>539</v>
+      </c>
+      <c r="G7" t="s">
+        <v>540</v>
+      </c>
+      <c r="H7" t="s">
+        <v>541</v>
+      </c>
+      <c r="I7" t="s">
+        <v>542</v>
+      </c>
+      <c r="J7" t="s">
+        <v>543</v>
+      </c>
+      <c r="K7" t="s">
+        <v>544</v>
+      </c>
+      <c r="L7" t="s">
+        <v>545</v>
+      </c>
+      <c r="M7" t="s">
+        <v>546</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>547</v>
+      </c>
+      <c r="C8" t="s">
+        <v>548</v>
+      </c>
+      <c r="D8" t="s">
+        <v>549</v>
+      </c>
+      <c r="E8" t="s">
+        <v>550</v>
+      </c>
+      <c r="F8" t="s">
+        <v>551</v>
+      </c>
+      <c r="G8" t="s">
+        <v>552</v>
+      </c>
+      <c r="H8" t="s">
+        <v>553</v>
+      </c>
+      <c r="I8" t="s">
+        <v>554</v>
+      </c>
+      <c r="J8" t="s">
+        <v>555</v>
+      </c>
+      <c r="K8" t="s">
+        <v>556</v>
+      </c>
+      <c r="L8" t="s">
+        <v>557</v>
+      </c>
+      <c r="M8" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>559</v>
+      </c>
+      <c r="C9" t="s">
+        <v>560</v>
+      </c>
+      <c r="D9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E9" t="s">
+        <v>562</v>
+      </c>
+      <c r="F9" t="s">
+        <v>563</v>
+      </c>
+      <c r="G9" t="s">
+        <v>564</v>
+      </c>
+      <c r="H9" t="s">
+        <v>565</v>
+      </c>
+      <c r="I9" t="s">
+        <v>566</v>
+      </c>
+      <c r="J9" t="s">
+        <v>567</v>
+      </c>
+      <c r="K9" t="s">
+        <v>568</v>
+      </c>
+      <c r="L9" t="s">
+        <v>569</v>
+      </c>
+      <c r="M9" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -4166,10 +6621,19 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4213,40 +6677,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D2" t="s">
+        <v>573</v>
+      </c>
+      <c r="E2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F2" t="s">
+        <v>575</v>
+      </c>
+      <c r="G2" t="s">
+        <v>576</v>
+      </c>
+      <c r="H2" t="s">
+        <v>577</v>
+      </c>
+      <c r="I2" t="s">
+        <v>578</v>
+      </c>
+      <c r="J2" t="s">
+        <v>579</v>
+      </c>
+      <c r="K2" t="s">
+        <v>580</v>
+      </c>
+      <c r="L2" t="s">
+        <v>581</v>
+      </c>
+      <c r="M2" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>583</v>
+      </c>
+      <c r="C3" t="s">
+        <v>584</v>
+      </c>
+      <c r="D3" t="s">
+        <v>585</v>
+      </c>
+      <c r="E3" t="s">
+        <v>586</v>
+      </c>
+      <c r="F3" t="s">
+        <v>587</v>
+      </c>
+      <c r="G3" t="s">
+        <v>588</v>
+      </c>
+      <c r="H3" t="s">
+        <v>589</v>
+      </c>
+      <c r="I3" t="s">
+        <v>590</v>
+      </c>
+      <c r="J3" t="s">
+        <v>591</v>
+      </c>
+      <c r="K3" t="s">
+        <v>592</v>
+      </c>
+      <c r="L3" t="s">
+        <v>593</v>
+      </c>
+      <c r="M3" t="s">
+        <v>594</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>595</v>
+      </c>
+      <c r="C4" t="s">
+        <v>596</v>
+      </c>
+      <c r="D4" t="s">
+        <v>597</v>
+      </c>
+      <c r="E4" t="s">
+        <v>598</v>
+      </c>
+      <c r="F4" t="s">
+        <v>599</v>
+      </c>
+      <c r="G4" t="s">
+        <v>600</v>
+      </c>
+      <c r="H4" t="s">
+        <v>601</v>
+      </c>
+      <c r="I4" t="s">
+        <v>602</v>
+      </c>
+      <c r="J4" t="s">
+        <v>603</v>
+      </c>
+      <c r="K4" t="s">
+        <v>604</v>
+      </c>
+      <c r="L4" t="s">
+        <v>605</v>
+      </c>
+      <c r="M4" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>607</v>
+      </c>
+      <c r="C5" t="s">
+        <v>608</v>
+      </c>
+      <c r="D5" t="s">
+        <v>609</v>
+      </c>
+      <c r="E5" t="s">
+        <v>610</v>
+      </c>
+      <c r="F5" t="s">
+        <v>611</v>
+      </c>
+      <c r="G5" t="s">
+        <v>612</v>
+      </c>
+      <c r="H5" t="s">
+        <v>613</v>
+      </c>
+      <c r="I5" t="s">
+        <v>614</v>
+      </c>
+      <c r="J5" t="s">
+        <v>615</v>
+      </c>
+      <c r="K5" t="s">
+        <v>616</v>
+      </c>
+      <c r="L5" t="s">
+        <v>617</v>
+      </c>
+      <c r="M5" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>619</v>
+      </c>
+      <c r="D6" t="s">
+        <v>620</v>
+      </c>
+      <c r="E6" t="s">
+        <v>621</v>
+      </c>
+      <c r="F6" t="s">
+        <v>622</v>
+      </c>
+      <c r="G6" t="s">
+        <v>623</v>
+      </c>
+      <c r="H6" t="s">
+        <v>624</v>
+      </c>
+      <c r="I6" t="s">
+        <v>625</v>
+      </c>
+      <c r="J6" t="s">
+        <v>626</v>
+      </c>
+      <c r="K6" t="s">
+        <v>627</v>
+      </c>
+      <c r="L6" t="s">
+        <v>628</v>
+      </c>
+      <c r="M6" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>630</v>
+      </c>
+      <c r="D7" t="s">
+        <v>631</v>
+      </c>
+      <c r="E7" t="s">
+        <v>632</v>
+      </c>
+      <c r="F7" t="s">
+        <v>633</v>
+      </c>
+      <c r="G7" t="s">
+        <v>634</v>
+      </c>
+      <c r="H7" t="s">
+        <v>635</v>
+      </c>
+      <c r="I7" t="s">
+        <v>636</v>
+      </c>
+      <c r="J7" t="s">
+        <v>637</v>
+      </c>
+      <c r="K7" t="s">
+        <v>638</v>
+      </c>
+      <c r="L7" t="s">
+        <v>639</v>
+      </c>
+      <c r="M7" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>641</v>
+      </c>
+      <c r="C8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D8" t="s">
+        <v>643</v>
+      </c>
+      <c r="E8" t="s">
+        <v>644</v>
+      </c>
+      <c r="F8" t="s">
+        <v>645</v>
+      </c>
+      <c r="G8" t="s">
+        <v>646</v>
+      </c>
+      <c r="H8" t="s">
+        <v>647</v>
+      </c>
+      <c r="I8" t="s">
+        <v>648</v>
+      </c>
+      <c r="J8" t="s">
+        <v>649</v>
+      </c>
+      <c r="K8" t="s">
+        <v>650</v>
+      </c>
+      <c r="L8" t="s">
+        <v>651</v>
+      </c>
+      <c r="M8" t="s">
+        <v>652</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>653</v>
+      </c>
+      <c r="C9" t="s">
+        <v>654</v>
+      </c>
+      <c r="D9" t="s">
+        <v>655</v>
+      </c>
+      <c r="E9" t="s">
+        <v>656</v>
+      </c>
+      <c r="F9" t="s">
+        <v>657</v>
+      </c>
+      <c r="G9" t="s">
+        <v>658</v>
+      </c>
+      <c r="H9" t="s">
+        <v>659</v>
+      </c>
+      <c r="I9" t="s">
+        <v>660</v>
+      </c>
+      <c r="J9" t="s">
+        <v>661</v>
+      </c>
+      <c r="K9" t="s">
+        <v>662</v>
+      </c>
+      <c r="L9" t="s">
+        <v>663</v>
+      </c>
+      <c r="M9" t="s">
+        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -4259,10 +7011,21 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4306,40 +7069,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>665</v>
+      </c>
+      <c r="C2" t="s">
+        <v>666</v>
+      </c>
+      <c r="D2" t="s">
+        <v>667</v>
+      </c>
+      <c r="E2" t="s">
+        <v>668</v>
+      </c>
+      <c r="F2" t="s">
+        <v>669</v>
+      </c>
+      <c r="G2" t="s">
+        <v>670</v>
+      </c>
+      <c r="H2" t="s">
+        <v>671</v>
+      </c>
+      <c r="I2" t="s">
+        <v>672</v>
+      </c>
+      <c r="J2" t="s">
+        <v>673</v>
+      </c>
+      <c r="K2" t="s">
+        <v>674</v>
+      </c>
+      <c r="L2" t="s">
+        <v>675</v>
+      </c>
+      <c r="M2" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>677</v>
+      </c>
+      <c r="C3" t="s">
+        <v>678</v>
+      </c>
+      <c r="D3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F3" t="s">
+        <v>681</v>
+      </c>
+      <c r="G3" t="s">
+        <v>682</v>
+      </c>
+      <c r="H3" t="s">
+        <v>683</v>
+      </c>
+      <c r="I3" t="s">
+        <v>684</v>
+      </c>
+      <c r="J3" t="s">
+        <v>685</v>
+      </c>
+      <c r="K3" t="s">
+        <v>686</v>
+      </c>
+      <c r="L3" t="s">
+        <v>687</v>
+      </c>
+      <c r="M3" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>689</v>
+      </c>
+      <c r="C4" t="s">
+        <v>690</v>
+      </c>
+      <c r="D4" t="s">
+        <v>691</v>
+      </c>
+      <c r="E4" t="s">
+        <v>692</v>
+      </c>
+      <c r="F4" t="s">
+        <v>693</v>
+      </c>
+      <c r="G4" t="s">
+        <v>694</v>
+      </c>
+      <c r="H4" t="s">
+        <v>695</v>
+      </c>
+      <c r="I4" t="s">
+        <v>696</v>
+      </c>
+      <c r="J4" t="s">
+        <v>697</v>
+      </c>
+      <c r="K4" t="s">
+        <v>698</v>
+      </c>
+      <c r="L4" t="s">
+        <v>699</v>
+      </c>
+      <c r="M4" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>701</v>
+      </c>
+      <c r="C5" t="s">
+        <v>702</v>
+      </c>
+      <c r="D5" t="s">
+        <v>703</v>
+      </c>
+      <c r="E5" t="s">
+        <v>704</v>
+      </c>
+      <c r="F5" t="s">
+        <v>705</v>
+      </c>
+      <c r="G5" t="s">
+        <v>706</v>
+      </c>
+      <c r="H5" t="s">
+        <v>707</v>
+      </c>
+      <c r="I5" t="s">
+        <v>708</v>
+      </c>
+      <c r="J5" t="s">
+        <v>709</v>
+      </c>
+      <c r="K5" t="s">
+        <v>710</v>
+      </c>
+      <c r="L5" t="s">
+        <v>711</v>
+      </c>
+      <c r="M5" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>713</v>
+      </c>
+      <c r="C6" t="s">
+        <v>714</v>
+      </c>
+      <c r="D6" t="s">
+        <v>715</v>
+      </c>
+      <c r="E6" t="s">
+        <v>716</v>
+      </c>
+      <c r="F6" t="s">
+        <v>717</v>
+      </c>
+      <c r="G6" t="s">
+        <v>718</v>
+      </c>
+      <c r="H6" t="s">
+        <v>719</v>
+      </c>
+      <c r="I6" t="s">
+        <v>720</v>
+      </c>
+      <c r="J6" t="s">
+        <v>721</v>
+      </c>
+      <c r="K6" t="s">
+        <v>722</v>
+      </c>
+      <c r="L6" t="s">
+        <v>723</v>
+      </c>
+      <c r="M6" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>725</v>
+      </c>
+      <c r="C7" t="s">
+        <v>726</v>
+      </c>
+      <c r="D7" t="s">
+        <v>727</v>
+      </c>
+      <c r="E7" t="s">
+        <v>728</v>
+      </c>
+      <c r="F7" t="s">
+        <v>729</v>
+      </c>
+      <c r="G7" t="s">
+        <v>730</v>
+      </c>
+      <c r="H7" t="s">
+        <v>731</v>
+      </c>
+      <c r="I7" t="s">
+        <v>732</v>
+      </c>
+      <c r="J7" t="s">
+        <v>733</v>
+      </c>
+      <c r="K7" t="s">
+        <v>734</v>
+      </c>
+      <c r="L7" t="s">
+        <v>735</v>
+      </c>
+      <c r="M7" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>737</v>
+      </c>
+      <c r="D8" t="s">
+        <v>738</v>
+      </c>
+      <c r="E8" t="s">
+        <v>739</v>
+      </c>
+      <c r="F8" t="s">
+        <v>740</v>
+      </c>
+      <c r="G8" t="s">
+        <v>741</v>
+      </c>
+      <c r="H8" t="s">
+        <v>742</v>
+      </c>
+      <c r="I8" t="s">
+        <v>743</v>
+      </c>
+      <c r="J8" t="s">
+        <v>744</v>
+      </c>
+      <c r="K8" t="s">
+        <v>745</v>
+      </c>
+      <c r="L8" t="s">
+        <v>746</v>
+      </c>
+      <c r="M8" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>748</v>
+      </c>
+      <c r="D9" t="s">
+        <v>749</v>
+      </c>
+      <c r="E9" t="s">
+        <v>750</v>
+      </c>
+      <c r="F9" t="s">
+        <v>751</v>
+      </c>
+      <c r="G9" t="s">
+        <v>752</v>
+      </c>
+      <c r="H9" t="s">
+        <v>753</v>
+      </c>
+      <c r="I9" t="s">
+        <v>754</v>
+      </c>
+      <c r="J9" t="s">
+        <v>755</v>
+      </c>
+      <c r="K9" t="s">
+        <v>756</v>
+      </c>
+      <c r="L9" t="s">
+        <v>757</v>
+      </c>
+      <c r="M9" t="s">
+        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -4352,10 +7403,21 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4399,40 +7461,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>759</v>
+      </c>
+      <c r="C2" t="s">
+        <v>760</v>
+      </c>
+      <c r="D2" t="s">
+        <v>761</v>
+      </c>
+      <c r="E2" t="s">
+        <v>762</v>
+      </c>
+      <c r="F2" t="s">
+        <v>763</v>
+      </c>
+      <c r="G2" t="s">
+        <v>764</v>
+      </c>
+      <c r="H2" t="s">
+        <v>765</v>
+      </c>
+      <c r="I2" t="s">
+        <v>766</v>
+      </c>
+      <c r="J2" t="s">
+        <v>767</v>
+      </c>
+      <c r="K2" t="s">
+        <v>768</v>
+      </c>
+      <c r="L2" t="s">
+        <v>769</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>770</v>
+      </c>
+      <c r="C3" t="s">
+        <v>771</v>
+      </c>
+      <c r="D3" t="s">
+        <v>772</v>
+      </c>
+      <c r="E3" t="s">
+        <v>773</v>
+      </c>
+      <c r="F3" t="s">
+        <v>774</v>
+      </c>
+      <c r="G3" t="s">
+        <v>775</v>
+      </c>
+      <c r="H3" t="s">
+        <v>776</v>
+      </c>
+      <c r="I3" t="s">
+        <v>777</v>
+      </c>
+      <c r="J3" t="s">
+        <v>778</v>
+      </c>
+      <c r="K3" t="s">
+        <v>779</v>
+      </c>
+      <c r="L3" t="s">
+        <v>780</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>781</v>
+      </c>
+      <c r="C4" t="s">
+        <v>782</v>
+      </c>
+      <c r="D4" t="s">
+        <v>783</v>
+      </c>
+      <c r="E4" t="s">
+        <v>784</v>
+      </c>
+      <c r="F4" t="s">
+        <v>785</v>
+      </c>
+      <c r="G4" t="s">
+        <v>786</v>
+      </c>
+      <c r="H4" t="s">
+        <v>787</v>
+      </c>
+      <c r="I4" t="s">
+        <v>788</v>
+      </c>
+      <c r="J4" t="s">
+        <v>789</v>
+      </c>
+      <c r="K4" t="s">
+        <v>790</v>
+      </c>
+      <c r="L4" t="s">
+        <v>791</v>
+      </c>
+      <c r="M4" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>793</v>
+      </c>
+      <c r="C5" t="s">
+        <v>794</v>
+      </c>
+      <c r="D5" t="s">
+        <v>795</v>
+      </c>
+      <c r="E5" t="s">
+        <v>796</v>
+      </c>
+      <c r="F5" t="s">
+        <v>797</v>
+      </c>
+      <c r="G5" t="s">
+        <v>798</v>
+      </c>
+      <c r="H5" t="s">
+        <v>799</v>
+      </c>
+      <c r="I5" t="s">
+        <v>800</v>
+      </c>
+      <c r="J5" t="s">
+        <v>801</v>
+      </c>
+      <c r="K5" t="s">
+        <v>802</v>
+      </c>
+      <c r="L5" t="s">
+        <v>803</v>
+      </c>
+      <c r="M5" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>805</v>
+      </c>
+      <c r="C6" t="s">
+        <v>806</v>
+      </c>
+      <c r="D6" t="s">
+        <v>807</v>
+      </c>
+      <c r="E6" t="s">
+        <v>808</v>
+      </c>
+      <c r="F6" t="s">
+        <v>809</v>
+      </c>
+      <c r="G6" t="s">
+        <v>810</v>
+      </c>
+      <c r="H6" t="s">
+        <v>811</v>
+      </c>
+      <c r="I6" t="s">
+        <v>812</v>
+      </c>
+      <c r="J6" t="s">
+        <v>813</v>
+      </c>
+      <c r="K6" t="s">
+        <v>814</v>
+      </c>
+      <c r="L6" t="s">
+        <v>815</v>
+      </c>
+      <c r="M6" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>817</v>
+      </c>
+      <c r="C7" t="s">
+        <v>818</v>
+      </c>
+      <c r="D7" t="s">
+        <v>819</v>
+      </c>
+      <c r="E7" t="s">
+        <v>820</v>
+      </c>
+      <c r="F7" t="s">
+        <v>821</v>
+      </c>
+      <c r="G7" t="s">
+        <v>822</v>
+      </c>
+      <c r="H7" t="s">
+        <v>823</v>
+      </c>
+      <c r="I7" t="s">
+        <v>824</v>
+      </c>
+      <c r="J7" t="s">
+        <v>825</v>
+      </c>
+      <c r="K7" t="s">
+        <v>826</v>
+      </c>
+      <c r="L7" t="s">
+        <v>827</v>
+      </c>
+      <c r="M7" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>829</v>
+      </c>
+      <c r="C8" t="s">
+        <v>830</v>
+      </c>
+      <c r="D8" t="s">
+        <v>831</v>
+      </c>
+      <c r="E8" t="s">
+        <v>832</v>
+      </c>
+      <c r="F8" t="s">
+        <v>833</v>
+      </c>
+      <c r="G8" t="s">
+        <v>834</v>
+      </c>
+      <c r="H8" t="s">
+        <v>835</v>
+      </c>
+      <c r="I8" t="s">
+        <v>836</v>
+      </c>
+      <c r="J8" t="s">
+        <v>837</v>
+      </c>
+      <c r="K8" t="s">
+        <v>838</v>
+      </c>
+      <c r="L8" t="s">
+        <v>839</v>
+      </c>
+      <c r="M8" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>841</v>
+      </c>
+      <c r="C9" t="s">
+        <v>842</v>
+      </c>
+      <c r="D9" t="s">
+        <v>843</v>
+      </c>
+      <c r="E9" t="s">
+        <v>844</v>
+      </c>
+      <c r="F9" t="s">
+        <v>845</v>
+      </c>
+      <c r="G9" t="s">
+        <v>846</v>
+      </c>
+      <c r="H9" t="s">
+        <v>847</v>
+      </c>
+      <c r="I9" t="s">
+        <v>848</v>
+      </c>
+      <c r="J9" t="s">
+        <v>849</v>
+      </c>
+      <c r="K9" t="s">
+        <v>850</v>
+      </c>
+      <c r="L9" t="s">
+        <v>851</v>
+      </c>
+      <c r="M9" t="s">
+        <v>852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change plate for RFLP analysis
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B1F84-2E4A-E149-88B7-16FF79A5C900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EB5909-CCBC-F64F-843D-28164D02992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36360" yWindow="-2440" windowWidth="22700" windowHeight="19540" firstSheet="4" activeTab="9" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="40540" yWindow="-2620" windowWidth="22700" windowHeight="19540" activeTab="4" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
     <sheet name="PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
     <sheet name="PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
     <sheet name="PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
-    <sheet name="PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
+    <sheet name="DONE PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
     <sheet name="PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
     <sheet name="PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
     <sheet name="PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
@@ -34,7 +34,7 @@
     <sheet name="PocHistone RLFP 022" sheetId="19" r:id="rId19"/>
     <sheet name="PocHistone RLFP 023" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3586,6 +3586,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3593,7 +3594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285077F4-FC02-8F44-91B5-576823D869B3}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3907,6 +3908,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4000,6 +4002,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4093,6 +4096,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4186,6 +4190,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4198,6 +4203,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4210,6 +4216,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4303,6 +4310,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4396,6 +4404,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4489,6 +4498,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4582,6 +4592,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4963,6 +4974,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5056,6 +5068,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5445,6 +5458,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5835,6 +5849,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5842,8 +5857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE14A41-7155-8342-8E24-88669BBABF7F}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6222,7 +6237,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -6231,7 +6247,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6613,6 +6629,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7003,6 +7020,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7395,6 +7413,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7787,5 +7806,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data to haplotype file
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EB5909-CCBC-F64F-843D-28164D02992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34FC548-6268-BC49-B98A-5E7598C09285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40540" yWindow="-2620" windowWidth="22700" windowHeight="19540" activeTab="4" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20200" activeTab="2" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
     <sheet name="PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
     <sheet name="PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
-    <sheet name="PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
+    <sheet name="DONE PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
     <sheet name="DONE PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
     <sheet name="PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
     <sheet name="PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="925">
   <si>
     <t>A</t>
   </si>
@@ -807,9 +807,6 @@
     <t>P6 F8 1090</t>
   </si>
   <si>
-    <t>P5 H1 1098</t>
-  </si>
-  <si>
     <t>P6 H12 1102</t>
   </si>
   <si>
@@ -918,9 +915,6 @@
     <t>P20 A4 1318</t>
   </si>
   <si>
-    <t>P19 A4 1321</t>
-  </si>
-  <si>
     <t>P17 A9 1325</t>
   </si>
   <si>
@@ -2827,6 +2821,15 @@
   </si>
   <si>
     <t xml:space="preserve">P30 </t>
+  </si>
+  <si>
+    <t>Plate needed:</t>
+  </si>
+  <si>
+    <t>Plate needed</t>
+  </si>
+  <si>
+    <t>P20 A2 1415</t>
   </si>
 </sst>
 </file>
@@ -2874,11 +2877,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3215,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D048908B-D0E1-4C43-91B7-69DE7A75BFD6}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3652,40 +3654,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>851</v>
+      </c>
+      <c r="C2" t="s">
+        <v>852</v>
+      </c>
+      <c r="D2" t="s">
         <v>853</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>854</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>855</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>856</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>857</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>858</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>859</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>860</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>861</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>862</v>
-      </c>
-      <c r="L2" t="s">
-        <v>863</v>
-      </c>
-      <c r="M2" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -3693,40 +3695,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>863</v>
+      </c>
+      <c r="C3" t="s">
+        <v>864</v>
+      </c>
+      <c r="D3" t="s">
         <v>865</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>866</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>867</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>868</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>869</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>870</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>871</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>872</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>873</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>874</v>
-      </c>
-      <c r="L3" t="s">
-        <v>875</v>
-      </c>
-      <c r="M3" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -3734,37 +3736,37 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>875</v>
+      </c>
+      <c r="C4" t="s">
+        <v>876</v>
+      </c>
+      <c r="D4" t="s">
         <v>877</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>878</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>879</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>880</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>881</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>882</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>883</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>884</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>885</v>
-      </c>
-      <c r="K4" t="s">
-        <v>886</v>
-      </c>
-      <c r="L4" t="s">
-        <v>887</v>
       </c>
       <c r="M4" t="s">
         <v>21</v>
@@ -3775,37 +3777,37 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>886</v>
+      </c>
+      <c r="C5" t="s">
+        <v>887</v>
+      </c>
+      <c r="D5" t="s">
         <v>888</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>889</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>890</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>891</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>892</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>893</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>894</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>895</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>896</v>
-      </c>
-      <c r="K5" t="s">
-        <v>897</v>
-      </c>
-      <c r="L5" t="s">
-        <v>898</v>
       </c>
       <c r="M5" t="s">
         <v>22</v>
@@ -3816,40 +3818,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>897</v>
+      </c>
+      <c r="C6" t="s">
+        <v>898</v>
+      </c>
+      <c r="D6" t="s">
         <v>899</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>900</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>901</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>902</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>903</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>904</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>905</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>906</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>907</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>908</v>
-      </c>
-      <c r="L6" t="s">
-        <v>909</v>
-      </c>
-      <c r="M6" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -3857,40 +3859,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>909</v>
+      </c>
+      <c r="C7" t="s">
+        <v>910</v>
+      </c>
+      <c r="D7" t="s">
         <v>911</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>912</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>913</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>914</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>915</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>916</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>917</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>918</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>919</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>920</v>
-      </c>
-      <c r="L7" t="s">
-        <v>921</v>
-      </c>
-      <c r="M7" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -3898,7 +3900,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -4598,10 +4600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA186EE-C9B2-1540-8F50-36A3B503B606}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="C1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4970,6 +4972,35 @@
       </c>
       <c r="M9" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>923</v>
+      </c>
+      <c r="B11">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="I11">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5074,15 +5105,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3646F6-6EE8-1E49-924E-2BFEEAA7CAE4}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -5312,22 +5343,22 @@
         <v>249</v>
       </c>
       <c r="G6" t="s">
+        <v>317</v>
+      </c>
+      <c r="H6" t="s">
         <v>250</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>251</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>252</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>253</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>254</v>
-      </c>
-      <c r="L6" t="s">
-        <v>255</v>
       </c>
       <c r="M6" t="s">
         <v>21</v>
@@ -5338,37 +5369,37 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
         <v>256</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>257</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>258</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>259</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>260</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>261</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>262</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>263</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>264</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>265</v>
-      </c>
-      <c r="L7" t="s">
-        <v>266</v>
       </c>
       <c r="M7" t="s">
         <v>22</v>
@@ -5379,40 +5410,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" t="s">
         <v>267</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>268</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>924</v>
+      </c>
+      <c r="F8" t="s">
         <v>269</v>
       </c>
-      <c r="E8" t="s">
-        <v>269</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>270</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>271</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>272</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>273</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>274</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>275</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>276</v>
-      </c>
-      <c r="M8" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -5420,40 +5451,69 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" t="s">
         <v>278</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>279</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>280</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>281</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>282</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>283</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>284</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>285</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>313</v>
+      </c>
+      <c r="L9" t="s">
         <v>286</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>287</v>
       </c>
-      <c r="L9" t="s">
-        <v>288</v>
-      </c>
-      <c r="M9" t="s">
-        <v>289</v>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <v>34</v>
+      </c>
+      <c r="H11">
+        <v>17</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5524,40 +5584,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
         <v>290</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>291</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>292</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>293</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>294</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>295</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>296</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>297</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>298</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>299</v>
-      </c>
-      <c r="L2" t="s">
-        <v>300</v>
-      </c>
-      <c r="M2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -5565,40 +5625,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D3" t="s">
         <v>302</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>303</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>304</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>305</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>306</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>307</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>308</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>309</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>310</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>311</v>
-      </c>
-      <c r="L3" t="s">
-        <v>312</v>
-      </c>
-      <c r="M3" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -5606,40 +5666,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" t="s">
         <v>314</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>315</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>316</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>317</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>318</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>319</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>320</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>321</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>322</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>323</v>
-      </c>
-      <c r="L4" t="s">
-        <v>324</v>
-      </c>
-      <c r="M4" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -5647,40 +5707,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" t="s">
         <v>326</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>327</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>328</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>329</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>330</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>331</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>332</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>333</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>334</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>335</v>
-      </c>
-      <c r="L5" t="s">
-        <v>336</v>
-      </c>
-      <c r="M5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -5688,40 +5748,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" t="s">
         <v>338</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>339</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>340</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>341</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>342</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>343</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>344</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>345</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>346</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>347</v>
-      </c>
-      <c r="L6" t="s">
-        <v>348</v>
-      </c>
-      <c r="M6" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -5729,40 +5789,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>348</v>
+      </c>
+      <c r="C7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D7" t="s">
         <v>350</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>351</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>352</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>353</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>354</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>355</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>356</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>357</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>358</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>359</v>
-      </c>
-      <c r="L7" t="s">
-        <v>360</v>
-      </c>
-      <c r="M7" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -5770,37 +5830,37 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>360</v>
+      </c>
+      <c r="C8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D8" t="s">
         <v>362</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>363</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>364</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>365</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>366</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>367</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>368</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>369</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>370</v>
-      </c>
-      <c r="K8" t="s">
-        <v>371</v>
-      </c>
-      <c r="L8" t="s">
-        <v>372</v>
       </c>
       <c r="M8" t="s">
         <v>21</v>
@@ -5811,37 +5871,37 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>371</v>
+      </c>
+      <c r="C9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" t="s">
         <v>373</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>374</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>375</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>376</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>377</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>378</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>379</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>380</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>381</v>
-      </c>
-      <c r="K9" t="s">
-        <v>382</v>
-      </c>
-      <c r="L9" t="s">
-        <v>383</v>
       </c>
       <c r="M9" t="s">
         <v>22</v>
@@ -5857,7 +5917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE14A41-7155-8342-8E24-88669BBABF7F}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -5916,37 +5976,37 @@
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -5957,37 +6017,37 @@
         <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -5995,40 +6055,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D4" t="s">
         <v>406</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>407</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>408</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>409</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>410</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>411</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>412</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" t="s">
         <v>413</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" t="s">
         <v>414</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" t="s">
         <v>415</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6036,40 +6096,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>416</v>
+      </c>
+      <c r="C5" t="s">
+        <v>417</v>
+      </c>
+      <c r="D5" t="s">
         <v>418</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>419</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>420</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>421</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>422</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>423</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>424</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="K5" t="s">
         <v>425</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" t="s">
         <v>426</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" t="s">
         <v>427</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>428</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -6077,40 +6137,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" t="s">
         <v>430</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>431</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>432</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>433</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>434</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>435</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>436</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="K6" t="s">
         <v>437</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" t="s">
         <v>438</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" t="s">
         <v>439</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -6118,40 +6178,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" t="s">
         <v>442</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>443</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>444</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>445</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>446</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>447</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>448</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="K7" t="s">
         <v>449</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="L7" t="s">
         <v>450</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="M7" t="s">
         <v>451</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -6159,40 +6219,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C8" t="s">
+        <v>453</v>
+      </c>
+      <c r="D8" t="s">
         <v>454</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>455</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>456</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>457</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>458</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>459</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>460</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" t="s">
         <v>461</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="L8" t="s">
         <v>462</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="M8" t="s">
         <v>463</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -6200,40 +6260,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>464</v>
+      </c>
+      <c r="C9" t="s">
+        <v>465</v>
+      </c>
+      <c r="D9" t="s">
         <v>466</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>467</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>468</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>469</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>470</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>471</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>472</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="K9" t="s">
         <v>473</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="L9" t="s">
         <v>474</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" t="s">
         <v>475</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -6304,40 +6364,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" t="s">
         <v>478</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>479</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>480</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>481</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>482</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>483</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>484</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>485</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>486</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>487</v>
-      </c>
-      <c r="L2" t="s">
-        <v>488</v>
-      </c>
-      <c r="M2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6345,40 +6405,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D3" t="s">
         <v>490</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>491</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>492</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>493</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>494</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>495</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>496</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>497</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>498</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>499</v>
-      </c>
-      <c r="L3" t="s">
-        <v>500</v>
-      </c>
-      <c r="M3" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6389,37 +6449,37 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
+        <v>500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>501</v>
+      </c>
+      <c r="E4" t="s">
         <v>502</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>503</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>504</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>505</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>506</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>507</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>508</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>509</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>510</v>
-      </c>
-      <c r="L4" t="s">
-        <v>511</v>
-      </c>
-      <c r="M4" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6430,37 +6490,37 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>511</v>
+      </c>
+      <c r="D5" t="s">
+        <v>512</v>
+      </c>
+      <c r="E5" t="s">
         <v>513</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>514</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>515</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>516</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>517</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>518</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>519</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>520</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>521</v>
-      </c>
-      <c r="L5" t="s">
-        <v>522</v>
-      </c>
-      <c r="M5" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -6468,40 +6528,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>522</v>
+      </c>
+      <c r="C6" t="s">
+        <v>523</v>
+      </c>
+      <c r="D6" t="s">
         <v>524</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>525</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>526</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>527</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>528</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>529</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>530</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
+        <v>530</v>
+      </c>
+      <c r="L6" t="s">
         <v>531</v>
       </c>
-      <c r="J6" t="s">
+      <c r="M6" t="s">
         <v>532</v>
-      </c>
-      <c r="K6" t="s">
-        <v>532</v>
-      </c>
-      <c r="L6" t="s">
-        <v>533</v>
-      </c>
-      <c r="M6" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -6509,40 +6569,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>533</v>
+      </c>
+      <c r="C7" t="s">
+        <v>534</v>
+      </c>
+      <c r="D7" t="s">
         <v>535</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>536</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>537</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>538</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>539</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>540</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>541</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>542</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>543</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>544</v>
-      </c>
-      <c r="L7" t="s">
-        <v>545</v>
-      </c>
-      <c r="M7" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -6550,40 +6610,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>545</v>
+      </c>
+      <c r="C8" t="s">
+        <v>546</v>
+      </c>
+      <c r="D8" t="s">
         <v>547</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>548</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>549</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>550</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>551</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>552</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>553</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>554</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>555</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>556</v>
-      </c>
-      <c r="L8" t="s">
-        <v>557</v>
-      </c>
-      <c r="M8" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -6591,40 +6651,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>557</v>
+      </c>
+      <c r="C9" t="s">
+        <v>558</v>
+      </c>
+      <c r="D9" t="s">
         <v>559</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>560</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>561</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>562</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>563</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>564</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>565</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>566</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>567</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>568</v>
-      </c>
-      <c r="L9" t="s">
-        <v>569</v>
-      </c>
-      <c r="M9" t="s">
-        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -6695,40 +6755,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>569</v>
+      </c>
+      <c r="C2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D2" t="s">
         <v>571</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>572</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>573</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>574</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>575</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>576</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>577</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>578</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>579</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>580</v>
-      </c>
-      <c r="L2" t="s">
-        <v>581</v>
-      </c>
-      <c r="M2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6736,40 +6796,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D3" t="s">
         <v>583</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>584</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>585</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>586</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>587</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>588</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>589</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>590</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>591</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>592</v>
-      </c>
-      <c r="L3" t="s">
-        <v>593</v>
-      </c>
-      <c r="M3" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6777,40 +6837,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>593</v>
+      </c>
+      <c r="C4" t="s">
+        <v>594</v>
+      </c>
+      <c r="D4" t="s">
         <v>595</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>596</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>597</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>598</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>599</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>600</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>601</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>602</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>603</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>604</v>
-      </c>
-      <c r="L4" t="s">
-        <v>605</v>
-      </c>
-      <c r="M4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6818,40 +6878,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D5" t="s">
         <v>607</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>608</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>609</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>610</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>611</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>612</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>613</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>614</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>615</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>616</v>
-      </c>
-      <c r="L5" t="s">
-        <v>617</v>
-      </c>
-      <c r="M5" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -6862,37 +6922,37 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
+        <v>617</v>
+      </c>
+      <c r="D6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E6" t="s">
         <v>619</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>620</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>621</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>622</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>623</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>624</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>625</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>626</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>627</v>
-      </c>
-      <c r="L6" t="s">
-        <v>628</v>
-      </c>
-      <c r="M6" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -6903,37 +6963,37 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>628</v>
+      </c>
+      <c r="D7" t="s">
+        <v>629</v>
+      </c>
+      <c r="E7" t="s">
         <v>630</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>631</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>632</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>633</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>634</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>635</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>636</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>637</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>638</v>
-      </c>
-      <c r="L7" t="s">
-        <v>639</v>
-      </c>
-      <c r="M7" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -6941,40 +7001,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>639</v>
+      </c>
+      <c r="C8" t="s">
+        <v>640</v>
+      </c>
+      <c r="D8" t="s">
         <v>641</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>642</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>643</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>644</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>645</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>646</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>647</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>648</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>649</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>650</v>
-      </c>
-      <c r="L8" t="s">
-        <v>651</v>
-      </c>
-      <c r="M8" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -6982,40 +7042,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>651</v>
+      </c>
+      <c r="C9" t="s">
+        <v>652</v>
+      </c>
+      <c r="D9" t="s">
         <v>653</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>654</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>655</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>656</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>657</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>658</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>659</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>660</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>661</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>662</v>
-      </c>
-      <c r="L9" t="s">
-        <v>663</v>
-      </c>
-      <c r="M9" t="s">
-        <v>664</v>
       </c>
     </row>
   </sheetData>
@@ -7029,7 +7089,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7088,40 +7148,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C2" t="s">
+        <v>664</v>
+      </c>
+      <c r="D2" t="s">
         <v>665</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>666</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>667</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>668</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>669</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>670</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>671</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>672</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>673</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>674</v>
-      </c>
-      <c r="L2" t="s">
-        <v>675</v>
-      </c>
-      <c r="M2" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -7129,40 +7189,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D3" t="s">
         <v>677</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>678</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>679</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>680</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>681</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>682</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>683</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>684</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>685</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>686</v>
-      </c>
-      <c r="L3" t="s">
-        <v>687</v>
-      </c>
-      <c r="M3" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -7170,40 +7230,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>687</v>
+      </c>
+      <c r="C4" t="s">
+        <v>688</v>
+      </c>
+      <c r="D4" t="s">
         <v>689</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>690</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>691</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>692</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>693</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>694</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>695</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>696</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>697</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>698</v>
-      </c>
-      <c r="L4" t="s">
-        <v>699</v>
-      </c>
-      <c r="M4" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -7211,40 +7271,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>699</v>
+      </c>
+      <c r="C5" t="s">
+        <v>700</v>
+      </c>
+      <c r="D5" t="s">
         <v>701</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>702</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>703</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>704</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>705</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>706</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>707</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>708</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>709</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>710</v>
-      </c>
-      <c r="L5" t="s">
-        <v>711</v>
-      </c>
-      <c r="M5" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -7252,40 +7312,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>711</v>
+      </c>
+      <c r="C6" t="s">
+        <v>712</v>
+      </c>
+      <c r="D6" t="s">
         <v>713</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>714</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>715</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>716</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>717</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>718</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>719</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>720</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>721</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>722</v>
-      </c>
-      <c r="L6" t="s">
-        <v>723</v>
-      </c>
-      <c r="M6" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -7293,40 +7353,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>723</v>
+      </c>
+      <c r="C7" t="s">
+        <v>724</v>
+      </c>
+      <c r="D7" t="s">
         <v>725</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>726</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>727</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>728</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>729</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>730</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>731</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>732</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>733</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>734</v>
-      </c>
-      <c r="L7" t="s">
-        <v>735</v>
-      </c>
-      <c r="M7" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -7337,37 +7397,37 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>735</v>
+      </c>
+      <c r="D8" t="s">
+        <v>736</v>
+      </c>
+      <c r="E8" t="s">
         <v>737</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>738</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>739</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>740</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>741</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>742</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>743</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>744</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>745</v>
-      </c>
-      <c r="L8" t="s">
-        <v>746</v>
-      </c>
-      <c r="M8" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -7378,37 +7438,37 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
+        <v>746</v>
+      </c>
+      <c r="D9" t="s">
+        <v>747</v>
+      </c>
+      <c r="E9" t="s">
         <v>748</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>749</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>750</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>751</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>752</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>753</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>754</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>755</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>756</v>
-      </c>
-      <c r="L9" t="s">
-        <v>757</v>
-      </c>
-      <c r="M9" t="s">
-        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -7422,7 +7482,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M3"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7481,37 +7541,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C2" t="s">
+        <v>758</v>
+      </c>
+      <c r="D2" t="s">
         <v>759</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>760</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>761</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>762</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>763</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>764</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>765</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>766</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>767</v>
-      </c>
-      <c r="K2" t="s">
-        <v>768</v>
-      </c>
-      <c r="L2" t="s">
-        <v>769</v>
       </c>
       <c r="M2" t="s">
         <v>21</v>
@@ -7522,37 +7582,37 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>768</v>
+      </c>
+      <c r="C3" t="s">
+        <v>769</v>
+      </c>
+      <c r="D3" t="s">
         <v>770</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>771</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>772</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>773</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>774</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>775</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>776</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>777</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>778</v>
-      </c>
-      <c r="K3" t="s">
-        <v>779</v>
-      </c>
-      <c r="L3" t="s">
-        <v>780</v>
       </c>
       <c r="M3" t="s">
         <v>22</v>
@@ -7563,40 +7623,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>779</v>
+      </c>
+      <c r="C4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D4" t="s">
         <v>781</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>782</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>783</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>784</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>785</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>786</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>787</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>788</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>789</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>790</v>
-      </c>
-      <c r="L4" t="s">
-        <v>791</v>
-      </c>
-      <c r="M4" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -7604,40 +7664,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>791</v>
+      </c>
+      <c r="C5" t="s">
+        <v>792</v>
+      </c>
+      <c r="D5" t="s">
         <v>793</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>794</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>795</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>796</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>797</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>798</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>799</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>800</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>801</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>802</v>
-      </c>
-      <c r="L5" t="s">
-        <v>803</v>
-      </c>
-      <c r="M5" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -7645,40 +7705,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>803</v>
+      </c>
+      <c r="C6" t="s">
+        <v>804</v>
+      </c>
+      <c r="D6" t="s">
         <v>805</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>806</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>807</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>808</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>809</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>810</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>811</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>812</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>813</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>814</v>
-      </c>
-      <c r="L6" t="s">
-        <v>815</v>
-      </c>
-      <c r="M6" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -7686,40 +7746,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>815</v>
+      </c>
+      <c r="C7" t="s">
+        <v>816</v>
+      </c>
+      <c r="D7" t="s">
         <v>817</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>818</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>819</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>820</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>821</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>822</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>823</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>824</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>825</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>826</v>
-      </c>
-      <c r="L7" t="s">
-        <v>827</v>
-      </c>
-      <c r="M7" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -7727,40 +7787,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>827</v>
+      </c>
+      <c r="C8" t="s">
+        <v>828</v>
+      </c>
+      <c r="D8" t="s">
         <v>829</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>830</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>831</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>832</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>833</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>834</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>835</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>836</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>837</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>838</v>
-      </c>
-      <c r="L8" t="s">
-        <v>839</v>
-      </c>
-      <c r="M8" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -7768,40 +7828,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>839</v>
+      </c>
+      <c r="C9" t="s">
+        <v>840</v>
+      </c>
+      <c r="D9" t="s">
         <v>841</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>842</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>843</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>844</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>845</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>846</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>847</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>848</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>849</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>850</v>
-      </c>
-      <c r="L9" t="s">
-        <v>851</v>
-      </c>
-      <c r="M9" t="s">
-        <v>852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add haplotype ID for 1a from the plate PocHistone RFLP 009
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34FC548-6268-BC49-B98A-5E7598C09285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD183BD4-CD1E-2840-B0FD-735DF4623BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20200" activeTab="2" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20140" activeTab="5" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
-    <sheet name="PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
-    <sheet name="PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
+    <sheet name="DONE PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
+    <sheet name="DONE PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
     <sheet name="DONE PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
     <sheet name="DONE PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
-    <sheet name="PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
+    <sheet name="DONE PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
     <sheet name="PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
     <sheet name="PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
     <sheet name="PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="925">
   <si>
     <t>A</t>
   </si>
@@ -4602,7 +4602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA186EE-C9B2-1540-8F50-36A3B503B606}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -5107,7 +5107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3646F6-6EE8-1E49-924E-2BFEEAA7CAE4}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -6306,8 +6306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB2FE5C-A0B9-AF47-B279-B32862A31F23}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6695,10 +6695,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A79109-2A37-B641-9D62-A5F755F5CB1D}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7078,6 +7078,52 @@
         <v>662</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>923</v>
+      </c>
+      <c r="B11">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>34</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+      <c r="G11">
+        <v>33</v>
+      </c>
+      <c r="H11">
+        <v>19</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>28</v>
+      </c>
+      <c r="K11">
+        <v>18</v>
+      </c>
+      <c r="L11">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7088,7 +7134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD62516-854B-1249-A94E-9B883C3B65BF}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating plate map for RFLP ID
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD183BD4-CD1E-2840-B0FD-735DF4623BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC18FC6-9E27-EB4D-A4A0-6B4A23938B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20140" activeTab="5" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" firstSheet="4" activeTab="12" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="DONE PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
     <sheet name="DONE PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
     <sheet name="DONE PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
-    <sheet name="PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
+    <sheet name="DONE PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
     <sheet name="PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
     <sheet name="PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
     <sheet name="PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
@@ -29,10 +29,6 @@
     <sheet name="PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
     <sheet name="PocHistone RLFP 018" sheetId="15" r:id="rId15"/>
     <sheet name="PocHistone RLFP 019" sheetId="16" r:id="rId16"/>
-    <sheet name="PocHistone RLFP 020" sheetId="17" r:id="rId17"/>
-    <sheet name="PocHistone RLFP 021" sheetId="18" r:id="rId18"/>
-    <sheet name="PocHistone RLFP 022" sheetId="19" r:id="rId19"/>
-    <sheet name="PocHistone RLFP 023" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="1170">
   <si>
     <t>A</t>
   </si>
@@ -2820,9 +2816,6 @@
     <t>P30 B7 2619</t>
   </si>
   <si>
-    <t xml:space="preserve">P30 </t>
-  </si>
-  <si>
     <t>Plate needed:</t>
   </si>
   <si>
@@ -2830,6 +2823,744 @@
   </si>
   <si>
     <t>P20 A2 1415</t>
+  </si>
+  <si>
+    <t>P12 E11 3872</t>
+  </si>
+  <si>
+    <t>P30 F7 2635</t>
+  </si>
+  <si>
+    <t>P30 B10 2636</t>
+  </si>
+  <si>
+    <t>P30 E8 2637</t>
+  </si>
+  <si>
+    <t>P30 G7 2638</t>
+  </si>
+  <si>
+    <t>P30 D12 2639</t>
+  </si>
+  <si>
+    <t>P30 E2 2640</t>
+  </si>
+  <si>
+    <t>P30 2645 E6</t>
+  </si>
+  <si>
+    <t>P30 C5 2647</t>
+  </si>
+  <si>
+    <t>P30 B9 2648</t>
+  </si>
+  <si>
+    <t>P30 C8 2649</t>
+  </si>
+  <si>
+    <t>P30 C7 2651</t>
+  </si>
+  <si>
+    <t>P30 D2 2652</t>
+  </si>
+  <si>
+    <t>P30 E3 2653</t>
+  </si>
+  <si>
+    <t>P30 C1 2656</t>
+  </si>
+  <si>
+    <t>P30 D8 2657</t>
+  </si>
+  <si>
+    <t>P30 D1 2658</t>
+  </si>
+  <si>
+    <t>P30 C2 2659</t>
+  </si>
+  <si>
+    <t>P30 E7 2661</t>
+  </si>
+  <si>
+    <t>P30 E4 2663</t>
+  </si>
+  <si>
+    <t>P30 G6 2664</t>
+  </si>
+  <si>
+    <t>P30 D9 2666</t>
+  </si>
+  <si>
+    <t>P30 C12 2673</t>
+  </si>
+  <si>
+    <t>P30 C3 2677</t>
+  </si>
+  <si>
+    <t>P30 F3 2680</t>
+  </si>
+  <si>
+    <t>P30 F6 2681</t>
+  </si>
+  <si>
+    <t>P27 F4 2688</t>
+  </si>
+  <si>
+    <t>P26 B6 2689</t>
+  </si>
+  <si>
+    <t>P27 D2 2691</t>
+  </si>
+  <si>
+    <t>P27 D9 2696</t>
+  </si>
+  <si>
+    <t>P27 H6 2698</t>
+  </si>
+  <si>
+    <t>P27 G6 2699</t>
+  </si>
+  <si>
+    <t>P27 H7 2701</t>
+  </si>
+  <si>
+    <t>P26 B2 2703</t>
+  </si>
+  <si>
+    <t>P27 G11 2704</t>
+  </si>
+  <si>
+    <t>P26 A2 2706</t>
+  </si>
+  <si>
+    <t>P26 B3 2711</t>
+  </si>
+  <si>
+    <t>P26 A12 2713</t>
+  </si>
+  <si>
+    <t>P26 A1 2715</t>
+  </si>
+  <si>
+    <t>P27 F6 2716</t>
+  </si>
+  <si>
+    <t>P27 H10 2717</t>
+  </si>
+  <si>
+    <t>P27 F9 2718</t>
+  </si>
+  <si>
+    <t>P26 A9 2719</t>
+  </si>
+  <si>
+    <t>P26 A5 2721</t>
+  </si>
+  <si>
+    <t>P27 G2 2722</t>
+  </si>
+  <si>
+    <t>P27 H9 2723</t>
+  </si>
+  <si>
+    <t>P26 A3 2727</t>
+  </si>
+  <si>
+    <t>P27 H5 2729</t>
+  </si>
+  <si>
+    <t>P27 F12 2731</t>
+  </si>
+  <si>
+    <t>P26 A11 2733</t>
+  </si>
+  <si>
+    <t>P27 H3 2734</t>
+  </si>
+  <si>
+    <t>P17 F10 2737</t>
+  </si>
+  <si>
+    <t>P25 C3 2740</t>
+  </si>
+  <si>
+    <t>P25 A8 2742</t>
+  </si>
+  <si>
+    <t>P25 C4 2747</t>
+  </si>
+  <si>
+    <t>P25 C7 2748</t>
+  </si>
+  <si>
+    <t>P25 A12 2752</t>
+  </si>
+  <si>
+    <t>P25 D10 2755</t>
+  </si>
+  <si>
+    <t>P25 E8 2764</t>
+  </si>
+  <si>
+    <t>P25 B9 2766</t>
+  </si>
+  <si>
+    <t>P25 E1 2771</t>
+  </si>
+  <si>
+    <t>P25 A10 2773</t>
+  </si>
+  <si>
+    <t>P25 C11 2777</t>
+  </si>
+  <si>
+    <t>P25 A11 2778</t>
+  </si>
+  <si>
+    <t>P25 D9 2779</t>
+  </si>
+  <si>
+    <t>P25 E9 2780</t>
+  </si>
+  <si>
+    <t>P25 B12 2781</t>
+  </si>
+  <si>
+    <t>P25 E2 2786</t>
+  </si>
+  <si>
+    <t>P25 B2 2787</t>
+  </si>
+  <si>
+    <t>P25 B4 2789</t>
+  </si>
+  <si>
+    <t>P17 F12 2793</t>
+  </si>
+  <si>
+    <t>P27 D10 2795</t>
+  </si>
+  <si>
+    <t>P27 D12 2798</t>
+  </si>
+  <si>
+    <t>P27 E10 2799</t>
+  </si>
+  <si>
+    <t>P27 D3 2800</t>
+  </si>
+  <si>
+    <t>P27 D1 2802</t>
+  </si>
+  <si>
+    <t>P27 E5 2804</t>
+  </si>
+  <si>
+    <t>P27 D4 2815</t>
+  </si>
+  <si>
+    <t>P27 E4 2816</t>
+  </si>
+  <si>
+    <t>P17 F7 2817</t>
+  </si>
+  <si>
+    <t>P27 E1 2819</t>
+  </si>
+  <si>
+    <t>P27 D11 2820</t>
+  </si>
+  <si>
+    <t>P27 F1 2821</t>
+  </si>
+  <si>
+    <t>P26 D5 2823</t>
+  </si>
+  <si>
+    <t>P26 G1 2827</t>
+  </si>
+  <si>
+    <t>P26 H5 2829</t>
+  </si>
+  <si>
+    <t>P25 A3 2830</t>
+  </si>
+  <si>
+    <t>P29 A3 2832</t>
+  </si>
+  <si>
+    <t>P29 A11 2833</t>
+  </si>
+  <si>
+    <t>P30 H11 2834</t>
+  </si>
+  <si>
+    <t>P26 E5 2838</t>
+  </si>
+  <si>
+    <t>P26 C6 2840</t>
+  </si>
+  <si>
+    <t>P26 C9 2841</t>
+  </si>
+  <si>
+    <t>P29 F3 2842</t>
+  </si>
+  <si>
+    <t>P26 C1 2845</t>
+  </si>
+  <si>
+    <t>P26 E1 2846</t>
+  </si>
+  <si>
+    <t>P26 G11 2848</t>
+  </si>
+  <si>
+    <t>P26 H8 2849</t>
+  </si>
+  <si>
+    <t>P26 F7 2850</t>
+  </si>
+  <si>
+    <t>P26 C7 2851</t>
+  </si>
+  <si>
+    <t>P26 F6 2853</t>
+  </si>
+  <si>
+    <t>P26 D10 2854</t>
+  </si>
+  <si>
+    <t>P29 B1 2855</t>
+  </si>
+  <si>
+    <t>P26 D3 2856</t>
+  </si>
+  <si>
+    <t>P26 F4 2857</t>
+  </si>
+  <si>
+    <t>P26 H10 2858</t>
+  </si>
+  <si>
+    <t>P26 B10 2861</t>
+  </si>
+  <si>
+    <t>P26 E2 2862</t>
+  </si>
+  <si>
+    <t>P26 H3 2863</t>
+  </si>
+  <si>
+    <t>P26 G6 2866</t>
+  </si>
+  <si>
+    <t>P26 D6 2867</t>
+  </si>
+  <si>
+    <t>P26 F9 2868</t>
+  </si>
+  <si>
+    <t>P26 C8 2869</t>
+  </si>
+  <si>
+    <t>P26 F1 2870</t>
+  </si>
+  <si>
+    <t>P25 A2 2871</t>
+  </si>
+  <si>
+    <t>P26 D7 2873</t>
+  </si>
+  <si>
+    <t>P26 B11 2875</t>
+  </si>
+  <si>
+    <t>P25 A1 2881</t>
+  </si>
+  <si>
+    <t>P26 C10 2883</t>
+  </si>
+  <si>
+    <t>P26 H11 2884</t>
+  </si>
+  <si>
+    <t>P26 G2 2885</t>
+  </si>
+  <si>
+    <t>P26 G7 2887</t>
+  </si>
+  <si>
+    <t>P26 D4 2889</t>
+  </si>
+  <si>
+    <t>P26 H2 2890</t>
+  </si>
+  <si>
+    <t>P26 E8 2891</t>
+  </si>
+  <si>
+    <t>P25 A4 2892</t>
+  </si>
+  <si>
+    <t>P26 H6 2894</t>
+  </si>
+  <si>
+    <t>P26 H9 2896</t>
+  </si>
+  <si>
+    <t>P26 C3 2898</t>
+  </si>
+  <si>
+    <t>P26 C11 2904</t>
+  </si>
+  <si>
+    <t>P26 D11 2909</t>
+  </si>
+  <si>
+    <t>P26 D9 2910</t>
+  </si>
+  <si>
+    <t>P24 C1 2912</t>
+  </si>
+  <si>
+    <t>P24 A10 2918</t>
+  </si>
+  <si>
+    <t>P23 C2 2919</t>
+  </si>
+  <si>
+    <t>P24 C6 2920</t>
+  </si>
+  <si>
+    <t>P23 B6 2921</t>
+  </si>
+  <si>
+    <t>P24 E1 2925</t>
+  </si>
+  <si>
+    <t>P24 C4 2926</t>
+  </si>
+  <si>
+    <t>P25 F6 2929</t>
+  </si>
+  <si>
+    <t>P24 H8 2931</t>
+  </si>
+  <si>
+    <t>P24 G2 2932</t>
+  </si>
+  <si>
+    <t>P24 E6 2933</t>
+  </si>
+  <si>
+    <t>P25 F7 2934</t>
+  </si>
+  <si>
+    <t>P26 G8 2936</t>
+  </si>
+  <si>
+    <t>P22 A3 2937</t>
+  </si>
+  <si>
+    <t>P25 G2 2938</t>
+  </si>
+  <si>
+    <t>P24 H7 2939</t>
+  </si>
+  <si>
+    <t>P25 G3 2941</t>
+  </si>
+  <si>
+    <t>P25 G4 2943</t>
+  </si>
+  <si>
+    <t>P24 F3 2946</t>
+  </si>
+  <si>
+    <t>P24 E8 2947</t>
+  </si>
+  <si>
+    <t>P24 G1 2950</t>
+  </si>
+  <si>
+    <t>P24 G11 2952</t>
+  </si>
+  <si>
+    <t>P25 G11 2953</t>
+  </si>
+  <si>
+    <t>P25 H9 2955</t>
+  </si>
+  <si>
+    <t>P29 B10 2957</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P30 H4 2958  </t>
+  </si>
+  <si>
+    <t>P30 H3 2959</t>
+  </si>
+  <si>
+    <t>P20 B2 2962</t>
+  </si>
+  <si>
+    <t>P29 A4 2967</t>
+  </si>
+  <si>
+    <t>P22 F6 2971</t>
+  </si>
+  <si>
+    <t>P22 E11 2974</t>
+  </si>
+  <si>
+    <t>P22 E7 2981</t>
+  </si>
+  <si>
+    <t>P22 F4 2982</t>
+  </si>
+  <si>
+    <t>P22 F3 2983</t>
+  </si>
+  <si>
+    <t>P22 E8 2988</t>
+  </si>
+  <si>
+    <t>P30 H8 2992</t>
+  </si>
+  <si>
+    <t>P30 H10 2993</t>
+  </si>
+  <si>
+    <t>P30 H1 2995</t>
+  </si>
+  <si>
+    <t>P29 D10 2997</t>
+  </si>
+  <si>
+    <t>P30 G8 2998</t>
+  </si>
+  <si>
+    <t>P22 G1 3002</t>
+  </si>
+  <si>
+    <t>P22 G5 3003</t>
+  </si>
+  <si>
+    <t>P22 F9 3011</t>
+  </si>
+  <si>
+    <t>P22 E10 3016</t>
+  </si>
+  <si>
+    <t>P22 G4 3033</t>
+  </si>
+  <si>
+    <t>P22 F7 3049</t>
+  </si>
+  <si>
+    <t>P22 G8 3050</t>
+  </si>
+  <si>
+    <t>P22 G6 3054</t>
+  </si>
+  <si>
+    <t>P22 G10 3058</t>
+  </si>
+  <si>
+    <t>P22 G9 3060</t>
+  </si>
+  <si>
+    <t>P22 F10 3063</t>
+  </si>
+  <si>
+    <t>P22 G3 3068</t>
+  </si>
+  <si>
+    <t>P20 H12 3076</t>
+  </si>
+  <si>
+    <t>P21 E4 3077</t>
+  </si>
+  <si>
+    <t>P21 E5 3078</t>
+  </si>
+  <si>
+    <t>P21 D4 3080</t>
+  </si>
+  <si>
+    <t>P20 H6 3081</t>
+  </si>
+  <si>
+    <t>P21 D7 3083</t>
+  </si>
+  <si>
+    <t>P21 F12 3084</t>
+  </si>
+  <si>
+    <t>P21 D1 3085</t>
+  </si>
+  <si>
+    <t>P21 H8 3086</t>
+  </si>
+  <si>
+    <t>P21 D10 3088</t>
+  </si>
+  <si>
+    <t>P21 D8 3096</t>
+  </si>
+  <si>
+    <t>P21 G11 3099</t>
+  </si>
+  <si>
+    <t>P21 F7 3100</t>
+  </si>
+  <si>
+    <t>P21 E6 3101</t>
+  </si>
+  <si>
+    <t>P21 C4 3103</t>
+  </si>
+  <si>
+    <t>P21 C6 3104</t>
+  </si>
+  <si>
+    <t>P21 G8 3105</t>
+  </si>
+  <si>
+    <t>P21 E7 3106</t>
+  </si>
+  <si>
+    <t>P21 H4 3107</t>
+  </si>
+  <si>
+    <t>P21 G7 3109</t>
+  </si>
+  <si>
+    <t>P21 G10 3110</t>
+  </si>
+  <si>
+    <t>P21 C1 3113</t>
+  </si>
+  <si>
+    <t>P21 G12 3114</t>
+  </si>
+  <si>
+    <t>P21 H6 3115</t>
+  </si>
+  <si>
+    <t>P21 H10 3116</t>
+  </si>
+  <si>
+    <t>P21 D3 3119</t>
+  </si>
+  <si>
+    <t>P21 E1 3121</t>
+  </si>
+  <si>
+    <t>P20 H8 3122</t>
+  </si>
+  <si>
+    <t>P13 A1 3123</t>
+  </si>
+  <si>
+    <t>P21 F1 3124</t>
+  </si>
+  <si>
+    <t>P21 H9 3125</t>
+  </si>
+  <si>
+    <t>P21 F4 3126</t>
+  </si>
+  <si>
+    <t>P21 D9 3127</t>
+  </si>
+  <si>
+    <t>P21 C11 3129</t>
+  </si>
+  <si>
+    <t>P21 C7 3130</t>
+  </si>
+  <si>
+    <t>P21 F10 3134</t>
+  </si>
+  <si>
+    <t>P21 H5 3135</t>
+  </si>
+  <si>
+    <t>P21 E10 3137</t>
+  </si>
+  <si>
+    <t>P21 C5 3138</t>
+  </si>
+  <si>
+    <t>P20 H11 3139</t>
+  </si>
+  <si>
+    <t>P21 H1 3144</t>
+  </si>
+  <si>
+    <t>P21 G3 3147</t>
+  </si>
+  <si>
+    <t>P23 F10 3150</t>
+  </si>
+  <si>
+    <t>P23 F3 3151</t>
+  </si>
+  <si>
+    <t>P23 G10 3153</t>
+  </si>
+  <si>
+    <t>P23 F7 3155</t>
+  </si>
+  <si>
+    <t>P23 G5 3157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P23 G4 3159 </t>
+  </si>
+  <si>
+    <t>P23 F4 3162</t>
+  </si>
+  <si>
+    <t>P21 H11 3165</t>
+  </si>
+  <si>
+    <t>P23 H8 3166</t>
+  </si>
+  <si>
+    <t>P21 G1 3167</t>
+  </si>
+  <si>
+    <t>P21 F9 3168</t>
+  </si>
+  <si>
+    <t>P21 E3 3169</t>
+  </si>
+  <si>
+    <t>P23 H9 3172</t>
+  </si>
+  <si>
+    <t>P22 H8 3174</t>
+  </si>
+  <si>
+    <t>P21 D5 3175</t>
+  </si>
+  <si>
+    <t>P23 F9 3178</t>
+  </si>
+  <si>
+    <t>P23 H4 3181</t>
+  </si>
+  <si>
+    <t>P23 E6 3184</t>
+  </si>
+  <si>
+    <t>P20 H5 3185</t>
+  </si>
+  <si>
+    <t>P23 E8 3185</t>
   </si>
 </sst>
 </file>
@@ -3218,10 +3949,15 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -3335,6 +4071,9 @@
       </c>
       <c r="K3" t="s">
         <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>924</v>
       </c>
       <c r="M3" t="s">
         <v>22</v>
@@ -3597,7 +4336,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="M4" sqref="M4:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3900,12 +4639,81 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>921</v>
+        <v>925</v>
+      </c>
+      <c r="C8" t="s">
+        <v>926</v>
+      </c>
+      <c r="D8" t="s">
+        <v>927</v>
+      </c>
+      <c r="E8" t="s">
+        <v>928</v>
+      </c>
+      <c r="F8" t="s">
+        <v>929</v>
+      </c>
+      <c r="G8" t="s">
+        <v>930</v>
+      </c>
+      <c r="H8" t="s">
+        <v>931</v>
+      </c>
+      <c r="I8" t="s">
+        <v>932</v>
+      </c>
+      <c r="J8" t="s">
+        <v>933</v>
+      </c>
+      <c r="K8" t="s">
+        <v>934</v>
+      </c>
+      <c r="L8" t="s">
+        <v>935</v>
+      </c>
+      <c r="M8" t="s">
+        <v>935</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>936</v>
+      </c>
+      <c r="C9" t="s">
+        <v>937</v>
+      </c>
+      <c r="D9" t="s">
+        <v>938</v>
+      </c>
+      <c r="E9" t="s">
+        <v>939</v>
+      </c>
+      <c r="F9" t="s">
+        <v>940</v>
+      </c>
+      <c r="G9" t="s">
+        <v>941</v>
+      </c>
+      <c r="H9" t="s">
+        <v>942</v>
+      </c>
+      <c r="I9" t="s">
+        <v>943</v>
+      </c>
+      <c r="J9" t="s">
+        <v>944</v>
+      </c>
+      <c r="K9" t="s">
+        <v>945</v>
+      </c>
+      <c r="L9" t="s">
+        <v>946</v>
+      </c>
+      <c r="M9" t="s">
+        <v>947</v>
       </c>
     </row>
   </sheetData>
@@ -3919,10 +4727,21 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -3966,40 +4785,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>948</v>
+      </c>
+      <c r="C2" t="s">
+        <v>949</v>
+      </c>
+      <c r="D2" t="s">
+        <v>950</v>
+      </c>
+      <c r="E2" t="s">
+        <v>951</v>
+      </c>
+      <c r="F2" t="s">
+        <v>952</v>
+      </c>
+      <c r="G2" t="s">
+        <v>953</v>
+      </c>
+      <c r="H2" t="s">
+        <v>954</v>
+      </c>
+      <c r="I2" t="s">
+        <v>955</v>
+      </c>
+      <c r="J2" t="s">
+        <v>956</v>
+      </c>
+      <c r="K2" t="s">
+        <v>957</v>
+      </c>
+      <c r="L2" t="s">
+        <v>958</v>
+      </c>
+      <c r="M2" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>960</v>
+      </c>
+      <c r="C3" t="s">
+        <v>961</v>
+      </c>
+      <c r="D3" t="s">
+        <v>962</v>
+      </c>
+      <c r="E3" t="s">
+        <v>963</v>
+      </c>
+      <c r="F3" t="s">
+        <v>964</v>
+      </c>
+      <c r="G3" t="s">
+        <v>965</v>
+      </c>
+      <c r="H3" t="s">
+        <v>966</v>
+      </c>
+      <c r="I3" t="s">
+        <v>967</v>
+      </c>
+      <c r="J3" t="s">
+        <v>968</v>
+      </c>
+      <c r="K3" t="s">
+        <v>969</v>
+      </c>
+      <c r="L3" t="s">
+        <v>970</v>
+      </c>
+      <c r="M3" t="s">
+        <v>971</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>972</v>
+      </c>
+      <c r="C4" t="s">
+        <v>973</v>
+      </c>
+      <c r="D4" t="s">
+        <v>974</v>
+      </c>
+      <c r="E4" t="s">
+        <v>975</v>
+      </c>
+      <c r="F4" t="s">
+        <v>976</v>
+      </c>
+      <c r="G4" t="s">
+        <v>977</v>
+      </c>
+      <c r="H4" t="s">
+        <v>978</v>
+      </c>
+      <c r="I4" t="s">
+        <v>979</v>
+      </c>
+      <c r="J4" t="s">
+        <v>980</v>
+      </c>
+      <c r="K4" t="s">
+        <v>981</v>
+      </c>
+      <c r="L4" t="s">
+        <v>982</v>
+      </c>
+      <c r="M4" t="s">
+        <v>983</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>984</v>
+      </c>
+      <c r="C5" t="s">
+        <v>985</v>
+      </c>
+      <c r="D5" t="s">
+        <v>986</v>
+      </c>
+      <c r="E5" t="s">
+        <v>987</v>
+      </c>
+      <c r="F5" t="s">
+        <v>988</v>
+      </c>
+      <c r="G5" t="s">
+        <v>989</v>
+      </c>
+      <c r="H5" t="s">
+        <v>990</v>
+      </c>
+      <c r="I5" t="s">
+        <v>991</v>
+      </c>
+      <c r="J5" t="s">
+        <v>992</v>
+      </c>
+      <c r="K5" t="s">
+        <v>993</v>
+      </c>
+      <c r="L5" t="s">
+        <v>994</v>
+      </c>
+      <c r="M5" t="s">
+        <v>995</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>996</v>
+      </c>
+      <c r="C6" t="s">
+        <v>997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1001</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1006</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1017</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1022</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1023</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1024</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1026</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1033</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1036</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1039</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1041</v>
       </c>
     </row>
   </sheetData>
@@ -4013,10 +5120,19 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4060,40 +5176,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1050</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1053</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1065</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1070</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1076</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1077</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1084</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1088</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1089</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1095</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1097</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1098</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1099</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1100</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1101</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1109</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1110</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1111</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1112</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1117</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1118</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1121</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1122</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1123</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1124</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1131</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1133</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1135</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4106,11 +5510,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A2B62E-D255-E642-9A27-CB767CFB6E84}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -4154,15 +5566,123 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1146</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1157</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1162</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1165</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1167</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1168</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1169</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -4227,289 +5747,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B70E42-AAE0-7749-8639-E9DF0FAC6835}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF91C3B2-23E8-DC4F-9294-C7687C1CC223}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA4BA05-9708-2142-AEC6-D0183FE10C6D}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4976,7 +6214,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B11">
         <v>37</v>
@@ -5001,100 +6239,6 @@
       </c>
       <c r="I11">
         <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40ED1F06-122F-9544-9F84-460B1A2D95E6}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5419,7 +6563,7 @@
         <v>268</v>
       </c>
       <c r="E8" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F8" t="s">
         <v>269</v>
@@ -5489,7 +6633,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -6306,7 +7450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB2FE5C-A0B9-AF47-B279-B32862A31F23}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -7080,7 +8224,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B11">
         <v>33</v>

</xml_diff>

<commit_message>
add all the RFLP to do
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC18FC6-9E27-EB4D-A4A0-6B4A23938B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762467F-8097-6C40-88A2-5A84644F1DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" firstSheet="4" activeTab="12" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20560" windowHeight="20200" firstSheet="11" activeTab="15" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1422">
   <si>
     <t>A</t>
   </si>
@@ -3561,6 +3561,762 @@
   </si>
   <si>
     <t>P23 E8 3185</t>
+  </si>
+  <si>
+    <t>P23 E11 3186</t>
+  </si>
+  <si>
+    <t>P21 H12 3188</t>
+  </si>
+  <si>
+    <t>P23 F1 3191</t>
+  </si>
+  <si>
+    <t>P22 H11 3192</t>
+  </si>
+  <si>
+    <t>P21 D6 3193</t>
+  </si>
+  <si>
+    <t>P23 H2 3195</t>
+  </si>
+  <si>
+    <t>P23 E4 3198</t>
+  </si>
+  <si>
+    <t>P21 H2 3201</t>
+  </si>
+  <si>
+    <t>P23 F6 3204</t>
+  </si>
+  <si>
+    <t>P22 H1 3206</t>
+  </si>
+  <si>
+    <t>P23 E9 3207</t>
+  </si>
+  <si>
+    <t>P23 G3 3208</t>
+  </si>
+  <si>
+    <t>P23 H1 3209</t>
+  </si>
+  <si>
+    <t>P23 G9 3210</t>
+  </si>
+  <si>
+    <t>P23 G2 3211</t>
+  </si>
+  <si>
+    <t>P23 G1 3214</t>
+  </si>
+  <si>
+    <t>P23 E10 3215</t>
+  </si>
+  <si>
+    <t>P21 G5 3216</t>
+  </si>
+  <si>
+    <t>P23 H5 3221</t>
+  </si>
+  <si>
+    <t>P20 H4 3224</t>
+  </si>
+  <si>
+    <t>P20 E5 3224</t>
+  </si>
+  <si>
+    <t>P22 B4 3225</t>
+  </si>
+  <si>
+    <t>P23 G11 3228</t>
+  </si>
+  <si>
+    <t>P23 H6 3230</t>
+  </si>
+  <si>
+    <t>P22 B1 3231</t>
+  </si>
+  <si>
+    <t>P22 C8 3232</t>
+  </si>
+  <si>
+    <t>P22 E1 3234</t>
+  </si>
+  <si>
+    <t>P22 E4 3235</t>
+  </si>
+  <si>
+    <t>P20 C8 3236</t>
+  </si>
+  <si>
+    <t>P20 C12 3237</t>
+  </si>
+  <si>
+    <t>P22 D10 3238</t>
+  </si>
+  <si>
+    <t>P20 D5 3241</t>
+  </si>
+  <si>
+    <t>P20 F5 3243</t>
+  </si>
+  <si>
+    <t>P20 D11 3246</t>
+  </si>
+  <si>
+    <t>P20 E8 3248</t>
+  </si>
+  <si>
+    <t>P20 G5 3250</t>
+  </si>
+  <si>
+    <t>P20 C11 3252</t>
+  </si>
+  <si>
+    <t>P22 C11 3254</t>
+  </si>
+  <si>
+    <t>P22 D5 3255</t>
+  </si>
+  <si>
+    <t>P22 B11 3256</t>
+  </si>
+  <si>
+    <t>P22 E2 3258</t>
+  </si>
+  <si>
+    <t>P22 C10 3263</t>
+  </si>
+  <si>
+    <t>P22 A10 3266</t>
+  </si>
+  <si>
+    <t>P22 D7 3268</t>
+  </si>
+  <si>
+    <t>P22 A5 3270</t>
+  </si>
+  <si>
+    <t>P22 B7 3271</t>
+  </si>
+  <si>
+    <t>P22 B2 3272</t>
+  </si>
+  <si>
+    <t>P22 C7 3274</t>
+  </si>
+  <si>
+    <t>P22 D9 3276</t>
+  </si>
+  <si>
+    <t>P22 B9 3277</t>
+  </si>
+  <si>
+    <t>P22 D2 3278</t>
+  </si>
+  <si>
+    <t>P22 A8 3280</t>
+  </si>
+  <si>
+    <t>P22 D8 3281</t>
+  </si>
+  <si>
+    <t>P22 C9 3283</t>
+  </si>
+  <si>
+    <t>P22 C5 3285</t>
+  </si>
+  <si>
+    <t>P22 D3 3286</t>
+  </si>
+  <si>
+    <t>P22 A4 3287</t>
+  </si>
+  <si>
+    <t>P22 D11 3288</t>
+  </si>
+  <si>
+    <t>P20 C6 3292</t>
+  </si>
+  <si>
+    <t>P20 C7 3293</t>
+  </si>
+  <si>
+    <t>P20 B4 3294</t>
+  </si>
+  <si>
+    <t>P20 D6 3298</t>
+  </si>
+  <si>
+    <t>P20 B6 3302</t>
+  </si>
+  <si>
+    <t>P20 F7 3303</t>
+  </si>
+  <si>
+    <t>P20 F4 3304</t>
+  </si>
+  <si>
+    <t>P20 E11 3305</t>
+  </si>
+  <si>
+    <t>P20 D7 3306</t>
+  </si>
+  <si>
+    <t>P20 D1 3310</t>
+  </si>
+  <si>
+    <t>P20 D3 3311</t>
+  </si>
+  <si>
+    <t>P20 C1 3314</t>
+  </si>
+  <si>
+    <t>P20 F8 3315</t>
+  </si>
+  <si>
+    <t>P20 D12 3316</t>
+  </si>
+  <si>
+    <t>P20 G2 3317</t>
+  </si>
+  <si>
+    <t>P20 E2 3318</t>
+  </si>
+  <si>
+    <t>P20 D2 3319</t>
+  </si>
+  <si>
+    <t>P20 F2 3320</t>
+  </si>
+  <si>
+    <t>P20 G3 3321</t>
+  </si>
+  <si>
+    <t>P20 H1 3325</t>
+  </si>
+  <si>
+    <t>P31 B12 3332</t>
+  </si>
+  <si>
+    <t>P20 C3 3333</t>
+  </si>
+  <si>
+    <t>P31 C8 3334</t>
+  </si>
+  <si>
+    <t>P31 D7 3335</t>
+  </si>
+  <si>
+    <t>P20 B5 3339</t>
+  </si>
+  <si>
+    <t>P20 B9 3340</t>
+  </si>
+  <si>
+    <t>P20 E7 3342</t>
+  </si>
+  <si>
+    <t>P20 F1 3343</t>
+  </si>
+  <si>
+    <t>P20 F12 3344</t>
+  </si>
+  <si>
+    <t>P20 C2 3346</t>
+  </si>
+  <si>
+    <t>P20 B11 3349</t>
+  </si>
+  <si>
+    <t>P23 C9 3354</t>
+  </si>
+  <si>
+    <t>P31 D8 3356</t>
+  </si>
+  <si>
+    <t>P23 D8 3357</t>
+  </si>
+  <si>
+    <t>P31 B2 3358</t>
+  </si>
+  <si>
+    <t>P31 C9 3361</t>
+  </si>
+  <si>
+    <t>P31 B7 3362</t>
+  </si>
+  <si>
+    <t>P31 C10 3363</t>
+  </si>
+  <si>
+    <t>P31 B1 3364</t>
+  </si>
+  <si>
+    <t>P31 C11 3365</t>
+  </si>
+  <si>
+    <t>P31 B8 3366</t>
+  </si>
+  <si>
+    <t>P31 C12 3367</t>
+  </si>
+  <si>
+    <t>P31 C6 3368</t>
+  </si>
+  <si>
+    <t>P23 D7 3370</t>
+  </si>
+  <si>
+    <t>P31 A4 3371</t>
+  </si>
+  <si>
+    <t>P23 D2 3372</t>
+  </si>
+  <si>
+    <t>P31 A7 3373</t>
+  </si>
+  <si>
+    <t>P31 C5 3374</t>
+  </si>
+  <si>
+    <t>P31 A12 3376</t>
+  </si>
+  <si>
+    <t>P30 B4 3377</t>
+  </si>
+  <si>
+    <t>P31 C3 3378</t>
+  </si>
+  <si>
+    <t>P31 E9 3380</t>
+  </si>
+  <si>
+    <t>P31 A8 3382</t>
+  </si>
+  <si>
+    <t>P31 B4 3383</t>
+  </si>
+  <si>
+    <t>P30 A7 3386</t>
+  </si>
+  <si>
+    <t>P23 D10 3387</t>
+  </si>
+  <si>
+    <t>P30 A4 3388</t>
+  </si>
+  <si>
+    <t>P23 D11 3390</t>
+  </si>
+  <si>
+    <t>P30 B1 3391</t>
+  </si>
+  <si>
+    <t>P31 A6 3392</t>
+  </si>
+  <si>
+    <t>P31 D5 3393</t>
+  </si>
+  <si>
+    <t>P31 E7 3394</t>
+  </si>
+  <si>
+    <t>P23 C12 3395</t>
+  </si>
+  <si>
+    <t>P23 C8 3396</t>
+  </si>
+  <si>
+    <t>P31 E4 3397</t>
+  </si>
+  <si>
+    <t>P31 B6 3398</t>
+  </si>
+  <si>
+    <t>P30 B5 3401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P31 E2 3403 </t>
+  </si>
+  <si>
+    <t>P23 C7 3404</t>
+  </si>
+  <si>
+    <t>P31 A5 3405</t>
+  </si>
+  <si>
+    <t>P31 D11 3406</t>
+  </si>
+  <si>
+    <t>P30 A1 3407</t>
+  </si>
+  <si>
+    <t>P31 D2 3409</t>
+  </si>
+  <si>
+    <t>P31 B5 3413</t>
+  </si>
+  <si>
+    <t>P31 E10 3414</t>
+  </si>
+  <si>
+    <t>P31 D10 3416</t>
+  </si>
+  <si>
+    <t>P30 A12 3417</t>
+  </si>
+  <si>
+    <t>P31 A9 3419</t>
+  </si>
+  <si>
+    <t>P23 E1 3421</t>
+  </si>
+  <si>
+    <t>P31 A10 3422</t>
+  </si>
+  <si>
+    <t>P31 E1 3423</t>
+  </si>
+  <si>
+    <t>P31 D6 3424</t>
+  </si>
+  <si>
+    <t>P31 D9 3425</t>
+  </si>
+  <si>
+    <t>P31 E6 3426</t>
+  </si>
+  <si>
+    <t>P30 A3 3427</t>
+  </si>
+  <si>
+    <t>P31 A2 3428</t>
+  </si>
+  <si>
+    <t>P31 C1 3431</t>
+  </si>
+  <si>
+    <t>P23 C11 3434</t>
+  </si>
+  <si>
+    <t>P23 D6 3435</t>
+  </si>
+  <si>
+    <t>P23 D9 3437</t>
+  </si>
+  <si>
+    <t>P23 E3 3439</t>
+  </si>
+  <si>
+    <t>P27 B7 3446</t>
+  </si>
+  <si>
+    <t>P27 A1 3447</t>
+  </si>
+  <si>
+    <t>P27 B8 3450</t>
+  </si>
+  <si>
+    <t>P27 B2 3451</t>
+  </si>
+  <si>
+    <t>P27 C7 3457</t>
+  </si>
+  <si>
+    <t>P28 A3 3458</t>
+  </si>
+  <si>
+    <t>P27 B5 3462</t>
+  </si>
+  <si>
+    <t>P28 D2 3463</t>
+  </si>
+  <si>
+    <t>P28 A7 3465</t>
+  </si>
+  <si>
+    <t>P23 D1 3466</t>
+  </si>
+  <si>
+    <t>P23 C5 3467</t>
+  </si>
+  <si>
+    <t>P31 B3 3468</t>
+  </si>
+  <si>
+    <t>P31 D12 3469</t>
+  </si>
+  <si>
+    <t>P31 C2 3470</t>
+  </si>
+  <si>
+    <t>P28 C9 3475</t>
+  </si>
+  <si>
+    <t>P27 A11 3476</t>
+  </si>
+  <si>
+    <t>P28 B5 3477</t>
+  </si>
+  <si>
+    <t>P27 A4 3478</t>
+  </si>
+  <si>
+    <t>P28 C7 3479</t>
+  </si>
+  <si>
+    <t>P28 D5 3481</t>
+  </si>
+  <si>
+    <t>P27 A3 3482</t>
+  </si>
+  <si>
+    <t>P24 C3 3484</t>
+  </si>
+  <si>
+    <t>P28 C3 3485</t>
+  </si>
+  <si>
+    <t>P27 A5 3488</t>
+  </si>
+  <si>
+    <t>P28 C5 3489</t>
+  </si>
+  <si>
+    <t>P28 B9 3490</t>
+  </si>
+  <si>
+    <t>P28 D11 3492</t>
+  </si>
+  <si>
+    <t>P28 C1 3494</t>
+  </si>
+  <si>
+    <t>P23 A8 3495</t>
+  </si>
+  <si>
+    <t>P24 A5 3497</t>
+  </si>
+  <si>
+    <t>P28 A9 3500</t>
+  </si>
+  <si>
+    <t>P24 D8 3505</t>
+  </si>
+  <si>
+    <t>P28 B3 3505</t>
+  </si>
+  <si>
+    <t>P24 A11 3508</t>
+  </si>
+  <si>
+    <t>P24 D2 3509</t>
+  </si>
+  <si>
+    <t>P24 A2 3510</t>
+  </si>
+  <si>
+    <t>P23 B7 3512</t>
+  </si>
+  <si>
+    <t>P24 C5 3514</t>
+  </si>
+  <si>
+    <t>P23 B2 3515</t>
+  </si>
+  <si>
+    <t>P24 B1 3516</t>
+  </si>
+  <si>
+    <t>P24 C8 3517</t>
+  </si>
+  <si>
+    <t>P23 C4 3518</t>
+  </si>
+  <si>
+    <t>P24 B9 3520</t>
+  </si>
+  <si>
+    <t>P28 D7 3521</t>
+  </si>
+  <si>
+    <t>P27 C4 3522</t>
+  </si>
+  <si>
+    <t>P23 B12 3523</t>
+  </si>
+  <si>
+    <t>P28 D10 3525</t>
+  </si>
+  <si>
+    <t>P28 C2 3526</t>
+  </si>
+  <si>
+    <t>P28 B12 3527</t>
+  </si>
+  <si>
+    <t>P27 A10 3528</t>
+  </si>
+  <si>
+    <t>P23 B4 3561</t>
+  </si>
+  <si>
+    <t>P24 D10 3562</t>
+  </si>
+  <si>
+    <t>P23 A3 3563</t>
+  </si>
+  <si>
+    <t>P24 A4 3566</t>
+  </si>
+  <si>
+    <t>P24 E2 3567</t>
+  </si>
+  <si>
+    <t>P24 D6 3568</t>
+  </si>
+  <si>
+    <t>P23 B9 3569</t>
+  </si>
+  <si>
+    <t>P23 C3 3572</t>
+  </si>
+  <si>
+    <t>P24 A3 3573</t>
+  </si>
+  <si>
+    <t>P24 B10 3574</t>
+  </si>
+  <si>
+    <t>P24 C3 3575</t>
+  </si>
+  <si>
+    <t>P24 D11 3576</t>
+  </si>
+  <si>
+    <t>P24 D12 3579</t>
+  </si>
+  <si>
+    <t>P23 B10 3582</t>
+  </si>
+  <si>
+    <t>P24 B6 3583</t>
+  </si>
+  <si>
+    <t>P24 D5 3585</t>
+  </si>
+  <si>
+    <t>P24 D1 3587</t>
+  </si>
+  <si>
+    <t>P23 B3 3589</t>
+  </si>
+  <si>
+    <t>P24 D4 3618</t>
+  </si>
+  <si>
+    <t>P23 A9 3619</t>
+  </si>
+  <si>
+    <t>P28 D6 3652</t>
+  </si>
+  <si>
+    <t>P27 B11 3653</t>
+  </si>
+  <si>
+    <t>P28 B10 3654</t>
+  </si>
+  <si>
+    <t>P27 C9 3655</t>
+  </si>
+  <si>
+    <t>P27 C6 3656</t>
+  </si>
+  <si>
+    <t>P28 C10 3658</t>
+  </si>
+  <si>
+    <t>P28 B6 3659</t>
+  </si>
+  <si>
+    <t>P27 B4 3660</t>
+  </si>
+  <si>
+    <t>P28 A5 3661</t>
+  </si>
+  <si>
+    <t>P28 B7 3662</t>
+  </si>
+  <si>
+    <t>P27 B10 3664</t>
+  </si>
+  <si>
+    <t>P27 A8 3665</t>
+  </si>
+  <si>
+    <t>P27 A7 3666</t>
+  </si>
+  <si>
+    <t>P28 A11 3669</t>
+  </si>
+  <si>
+    <t>P28 A10 3671</t>
+  </si>
+  <si>
+    <t>P28 C8 3675</t>
+  </si>
+  <si>
+    <t>P28 C4 3676</t>
+  </si>
+  <si>
+    <t>P28 D8 3678</t>
+  </si>
+  <si>
+    <t>P12 C3 3721</t>
+  </si>
+  <si>
+    <t>P14 A11 3729</t>
+  </si>
+  <si>
+    <t>P15 C3 3738</t>
+  </si>
+  <si>
+    <t>P15 A7 3752</t>
+  </si>
+  <si>
+    <t>P15 C7 3884</t>
+  </si>
+  <si>
+    <t>P38 C12 3894</t>
+  </si>
+  <si>
+    <t>P38 C8 3898</t>
+  </si>
+  <si>
+    <t>P38 D2 3900</t>
+  </si>
+  <si>
+    <t>P38 D4 3910</t>
+  </si>
+  <si>
+    <t>P12 G4 3919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P38 D7 3928 </t>
+  </si>
+  <si>
+    <t>P38 D9 3930</t>
+  </si>
+  <si>
+    <t>P38 C9 3936</t>
+  </si>
+  <si>
+    <t>P12 C10 3751</t>
+  </si>
+  <si>
+    <t>P38 C11 3789</t>
   </si>
 </sst>
 </file>
@@ -3949,7 +4705,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3957,6 +4713,7 @@
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -5510,16 +6267,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A2B62E-D255-E642-9A27-CB767CFB6E84}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5689,25 +6450,205 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1175</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1176</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1177</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1178</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1179</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1180</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1181</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1186</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1188</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1190</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1191</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1192</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1193</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1201</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1202</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1203</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1204</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1205</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1209</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1212</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1213</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1215</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1217</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1223</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1224</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1225</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1226</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1228</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1229</v>
       </c>
     </row>
   </sheetData>
@@ -5718,12 +6659,389 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC92E7F-C385-B444-97EB-2FAF7E405F1D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1235</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1237</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1262</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1263</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1270</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1271</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1282</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1283</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1284</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1285</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1286</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1295</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1296</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1297</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1298</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1303</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1304</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1306</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1307</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1308</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1309</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1310</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1316</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1317</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1318</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1319</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1320</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1321</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1322</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5731,12 +7049,392 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA46985-9500-3F4A-B310-368C14889727}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1330</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1332</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1333</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1334</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1347</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1348</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1350</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1351</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1352</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1353</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1354</v>
+      </c>
+      <c r="K4" t="s">
+        <v>1355</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1356</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1360</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1361</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1362</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1363</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1366</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1367</v>
+      </c>
+      <c r="L5" t="s">
+        <v>1368</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1371</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1376</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1377</v>
+      </c>
+      <c r="K6" t="s">
+        <v>1378</v>
+      </c>
+      <c r="L6" t="s">
+        <v>1379</v>
+      </c>
+      <c r="M6" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1381</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1383</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1385</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1386</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1387</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1388</v>
+      </c>
+      <c r="K7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1390</v>
+      </c>
+      <c r="M7" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1398</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1399</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1400</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1401</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1402</v>
+      </c>
+      <c r="M8" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1407</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1409</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1410</v>
+      </c>
+      <c r="I9" t="s">
+        <v>924</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1411</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1412</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1413</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5744,13 +7442,18 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE75D2-5269-B646-8E1B-9E77EE40A1CD}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1">
@@ -5794,40 +7497,67 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1415</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1418</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="J2" t="s">
+        <v>269</v>
+      </c>
+      <c r="K2" t="s">
+        <v>534</v>
+      </c>
+      <c r="L2" t="s">
+        <v>537</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
+      <c r="B3" t="s">
+        <v>924</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G3" t="s">
+        <v>534</v>
+      </c>
+      <c r="H3" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update RFLP plate file
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762467F-8097-6C40-88A2-5A84644F1DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DE7F6-18C9-3C4E-BB78-81B7868AC8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20560" windowHeight="20200" firstSheet="11" activeTab="15" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20200" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="1423">
   <si>
     <t>A</t>
   </si>
@@ -4317,6 +4317,9 @@
   </si>
   <si>
     <t>P38 C11 3789</t>
+  </si>
+  <si>
+    <t>plate needed</t>
   </si>
 </sst>
 </file>
@@ -4702,10 +4705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D048908B-D0E1-4C43-91B7-69DE7A75BFD6}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5080,6 +5083,44 @@
       </c>
       <c r="M9" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B11">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>37</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -7052,7 +7093,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7444,7 +7485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE75D2-5269-B646-8E1B-9E77EE40A1CD}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -10009,7 +10050,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="B21" sqref="B21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update RFLP plate maps
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DE7F6-18C9-3C4E-BB78-81B7868AC8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FD3A69-3F56-804A-A5BD-477FDA4BC3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20200" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20200" firstSheet="9" activeTab="15" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
-    <sheet name="PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
+    <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
     <sheet name="DONE PocHistone RLFP 005" sheetId="2" r:id="rId2"/>
     <sheet name="DONE PocHistone RLFP 006" sheetId="3" r:id="rId3"/>
     <sheet name="DONE PocHistone RLFP 007" sheetId="4" r:id="rId4"/>
@@ -4707,7 +4707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D048908B-D0E1-4C43-91B7-69DE7A75BFD6}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -7485,7 +7485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE75D2-5269-B646-8E1B-9E77EE40A1CD}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add data for halotype 1a
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC34A44-2DE2-9247-AB89-E0F7B5F84C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9427D76A-7DF7-2144-A133-1142C1F820A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="3" activeTab="7" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="5" activeTab="8" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="DONE PocHistone RLFP 008" sheetId="5" r:id="rId5"/>
     <sheet name="DONE PocHistone RLFP 009" sheetId="6" r:id="rId6"/>
     <sheet name="DONE PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
-    <sheet name="PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
+    <sheet name="DONE PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
     <sheet name="PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
     <sheet name="PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
     <sheet name="PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1424">
   <si>
     <t>A</t>
   </si>
@@ -10052,7 +10052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD62516-854B-1249-A94E-9B883C3B65BF}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -10470,10 +10470,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A32ED-889B-7C45-930B-67D659BB3C81}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10855,6 +10855,32 @@
         <v>850</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B11">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update file with RFLP plate
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9427D76A-7DF7-2144-A133-1142C1F820A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C723570-0D36-CD4B-ABA4-E777E1E72BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="5" activeTab="8" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="5" activeTab="10" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="1424">
   <si>
     <t>A</t>
   </si>
@@ -5134,10 +5134,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{285077F4-FC02-8F44-91B5-576823D869B3}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M5"/>
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5517,6 +5517,35 @@
         <v>947</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>26</v>
+      </c>
+      <c r="H11">
+        <v>27</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -5525,10 +5554,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45504A04-9B98-C942-A0B3-87EEDCC114F4}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5908,6 +5937,29 @@
       </c>
       <c r="M9" t="s">
         <v>1041</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>26</v>
+      </c>
+      <c r="E11">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -10472,7 +10524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE5A32ED-889B-7C45-930B-67D659BB3C81}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add data from plate PocHistone RFLP 012
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B284EB-77B7-074A-8784-F0C4F31838F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6FA896-46A2-C84A-B872-80B21852D779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="9" activeTab="12" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1424">
   <si>
     <t>A</t>
   </si>
@@ -5970,10 +5970,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF91483-CA2D-194B-9E9C-0698B90E3C5F}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6351,6 +6351,38 @@
       </c>
       <c r="M9" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add plate pochistone RFLP 014 to haplotype species identification
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6FA896-46A2-C84A-B872-80B21852D779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9AD420-628E-9841-B588-76FC6EEF15B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="9" activeTab="12" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="8" activeTab="11" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -22,8 +22,8 @@
     <sheet name="DONE PocHistone RLFP 010" sheetId="7" r:id="rId7"/>
     <sheet name="DONE PocHistone RLFP 011" sheetId="8" r:id="rId8"/>
     <sheet name="DONE PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
-    <sheet name="PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
-    <sheet name="PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
+    <sheet name="DONE PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
+    <sheet name="DONE PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
     <sheet name="PocHistone RLFP 015" sheetId="12" r:id="rId12"/>
     <sheet name="PocHistone RLFP 016" sheetId="13" r:id="rId13"/>
     <sheet name="PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1424">
   <si>
     <t>A</t>
   </si>
@@ -5972,7 +5972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF91483-CA2D-194B-9E9C-0698B90E3C5F}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -6393,10 +6393,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A2B62E-D255-E642-9A27-CB767CFB6E84}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6777,6 +6777,26 @@
       </c>
       <c r="M9" t="s">
         <v>1229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -7573,7 +7593,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add ID species from plate PocHistone 015
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF9AD420-628E-9841-B588-76FC6EEF15B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C26EA0-1728-2745-ACCF-AFBB98AF6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="8" activeTab="11" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="9" activeTab="11" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="DONE PocHistone RLFP 012" sheetId="9" r:id="rId9"/>
     <sheet name="DONE PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
     <sheet name="DONE PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
-    <sheet name="PocHistone RLFP 015" sheetId="12" r:id="rId12"/>
+    <sheet name="DONE PocHistone RLFP 015" sheetId="12" r:id="rId12"/>
     <sheet name="PocHistone RLFP 016" sheetId="13" r:id="rId13"/>
     <sheet name="PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
     <sheet name="PocHistone RLFP 018" sheetId="15" r:id="rId15"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1424">
   <si>
     <t>A</t>
   </si>
@@ -6807,10 +6807,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC92E7F-C385-B444-97EB-2FAF7E405F1D}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7189,6 +7189,26 @@
         <v>1323</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7197,10 +7217,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA46985-9500-3F4A-B310-368C14889727}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7580,6 +7600,38 @@
       </c>
       <c r="M9" t="s">
         <v>1414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>922</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <v>31</v>
+      </c>
+      <c r="F11">
+        <v>28</v>
+      </c>
+      <c r="G11">
+        <v>24</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add last plast of pochistone 019
</commit_message>
<xml_diff>
--- a/Data/20250717_RFLP_PLATE.xlsx
+++ b/Data/20250717_RFLP_PLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrickharnay/Documents/MyProjects/Pocillopora-Lagoon-Abundance/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C26EA0-1728-2745-ACCF-AFBB98AF6F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAD8A53-F0F4-024B-BF3A-24AFD01885B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="26040" windowHeight="20180" firstSheet="9" activeTab="11" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
+    <workbookView xWindow="4360" yWindow="980" windowWidth="20720" windowHeight="20180" firstSheet="10" activeTab="15" xr2:uid="{A601EE7E-9C1F-5246-AD58-1BA19970A352}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE PocHistone RLFP 004" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
     <sheet name="DONE PocHistone RLFP 013" sheetId="10" r:id="rId10"/>
     <sheet name="DONE PocHistone RLFP 014" sheetId="11" r:id="rId11"/>
     <sheet name="DONE PocHistone RLFP 015" sheetId="12" r:id="rId12"/>
-    <sheet name="PocHistone RLFP 016" sheetId="13" r:id="rId13"/>
-    <sheet name="PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
-    <sheet name="PocHistone RLFP 018" sheetId="15" r:id="rId15"/>
+    <sheet name="DONE PocHistone RLFP 016" sheetId="13" r:id="rId13"/>
+    <sheet name="DONE PocHistone RLFP 017" sheetId="14" r:id="rId14"/>
+    <sheet name="DONE PocHistone RLFP 018" sheetId="15" r:id="rId15"/>
     <sheet name="PocHistone RLFP 019" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1612" uniqueCount="1439">
   <si>
     <t>A</t>
   </si>
@@ -4304,25 +4304,70 @@
     <t>P12 G4 3919</t>
   </si>
   <si>
-    <t xml:space="preserve">P38 D7 3928 </t>
-  </si>
-  <si>
-    <t>P38 D9 3930</t>
-  </si>
-  <si>
     <t>P38 C9 3936</t>
   </si>
   <si>
-    <t>P12 C10 3751</t>
-  </si>
-  <si>
-    <t>P38 C11 3789</t>
-  </si>
-  <si>
     <t>plate needed</t>
   </si>
   <si>
     <t>1 (possitif) C2</t>
+  </si>
+  <si>
+    <t>P13 D11 613</t>
+  </si>
+  <si>
+    <t>P5 G8 760</t>
+  </si>
+  <si>
+    <t>P37 G9 802</t>
+  </si>
+  <si>
+    <t>P6 F6 1011</t>
+  </si>
+  <si>
+    <t>P5 H1 1098</t>
+  </si>
+  <si>
+    <t>P19 A4 1321</t>
+  </si>
+  <si>
+    <t>P19 C1 1418</t>
+  </si>
+  <si>
+    <t>P16 H4 1444</t>
+  </si>
+  <si>
+    <t>P35 A11 1456</t>
+  </si>
+  <si>
+    <t>P34 C8 1514</t>
+  </si>
+  <si>
+    <t>P29 H8 2437</t>
+  </si>
+  <si>
+    <t>P29 C10 2604</t>
+  </si>
+  <si>
+    <t>P30 E10 2676</t>
+  </si>
+  <si>
+    <t>P21 F6 3102</t>
+  </si>
+  <si>
+    <t>P20 F11 3242</t>
+  </si>
+  <si>
+    <t>P24 A9 3507</t>
+  </si>
+  <si>
+    <t>P38 D7 3928</t>
+  </si>
+  <si>
+    <t>P38 D9 3830</t>
+  </si>
+  <si>
+    <t>P38 D11 3940</t>
   </si>
 </sst>
 </file>
@@ -5090,7 +5135,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="B11">
         <v>31</v>
@@ -5972,7 +6017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF91483-CA2D-194B-9E9C-0698B90E3C5F}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -7642,10 +7687,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCE75D2-5269-B646-8E1B-9E77EE40A1CD}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7653,6 +7698,8 @@
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -7701,37 +7748,37 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>1415</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>1416</v>
+        <v>1420</v>
       </c>
       <c r="F2" t="s">
-        <v>1417</v>
+        <v>1421</v>
       </c>
       <c r="G2" t="s">
-        <v>1418</v>
+        <v>1422</v>
       </c>
       <c r="H2" t="s">
-        <v>1418</v>
+        <v>1423</v>
       </c>
       <c r="I2" t="s">
-        <v>1419</v>
+        <v>1424</v>
       </c>
       <c r="J2" t="s">
+        <v>1438</v>
+      </c>
+      <c r="K2" t="s">
         <v>269</v>
       </c>
-      <c r="K2" t="s">
-        <v>534</v>
-      </c>
       <c r="L2" t="s">
-        <v>537</v>
+        <v>1425</v>
       </c>
       <c r="M2" t="s">
-        <v>51</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -7739,25 +7786,81 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>924</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G3" t="s">
+        <v>461</v>
+      </c>
+      <c r="H3" t="s">
+        <v>534</v>
+      </c>
+      <c r="I3" t="s">
+        <v>537</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="K3" t="s">
+        <v>891</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1433</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1349</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1435</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1367</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1408</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1415</v>
+      </c>
+      <c r="J4" t="s">
         <v>1416</v>
       </c>
-      <c r="D3" t="s">
-        <v>1408</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1420</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1421</v>
-      </c>
-      <c r="G3" t="s">
-        <v>534</v>
-      </c>
-      <c r="H3" t="s">
-        <v>537</v>
+      <c r="K4" t="s">
+        <v>1436</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1437</v>
+      </c>
+      <c r="M4" t="s">
+        <v>1417</v>
       </c>
     </row>
   </sheetData>
@@ -10615,7 +10718,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
     </row>
   </sheetData>
@@ -11013,7 +11116,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
       <c r="B11">
         <v>18</v>

</xml_diff>